<commit_message>
Lenovo Ideapad 320, Checkin Timestamp :: Sun 06/26/2022-13:41:50.17;
</commit_message>
<xml_diff>
--- a/My Transformation Journey.xlsx
+++ b/My Transformation Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nc\Awakening-The-Giant-Naresh-Chaurasia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFBA47D-F9CE-458A-9588-995CDC9528B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DE45CF-4DC6-4FD7-B998-0398644F8AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="4" xr2:uid="{45287DFE-D99B-4274-A6CA-7DF7915FBBA5}"/>
   </bookViews>
@@ -1771,14 +1771,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1818,6 +1812,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1921,6 +1921,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1930,15 +1933,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1946,6 +1940,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1976,6 +1976,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1983,15 +1992,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2003,6 +2003,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2010,15 +2019,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2274,25 +2274,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2594,25 +2585,25 @@
                 <c:formatCode>dd\ mmm</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44725</c:v>
+                  <c:v>44732</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44726</c:v>
+                  <c:v>44733</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44727</c:v>
+                  <c:v>44734</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44728</c:v>
+                  <c:v>44735</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44729</c:v>
+                  <c:v>44736</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44730</c:v>
+                  <c:v>44737</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44731</c:v>
+                  <c:v>44738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2624,13 +2615,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2901,12 +2892,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11534,7 +11519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A659E6A-7EE0-4249-A963-0689D0721EB6}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -12828,7 +12813,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -12847,7 +12832,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="145"/>
+      <c r="A2" s="146"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -12864,7 +12849,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="146"/>
+      <c r="A3" s="147"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -12922,7 +12907,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="147"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="18" t="s">
         <v>29</v>
       </c>
@@ -13002,7 +12987,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="147"/>
+      <c r="A7" s="144"/>
       <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
@@ -13082,7 +13067,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="144"/>
+      <c r="A9" s="145"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -13162,7 +13147,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="144"/>
+      <c r="A11" s="145"/>
       <c r="B11" s="18" t="s">
         <v>29</v>
       </c>
@@ -13242,7 +13227,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="144"/>
+      <c r="A13" s="145"/>
       <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
@@ -13322,7 +13307,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
+      <c r="A15" s="145"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -13402,7 +13387,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="144"/>
+      <c r="A17" s="145"/>
       <c r="B17" s="18" t="s">
         <v>29</v>
       </c>
@@ -13482,7 +13467,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="147"/>
+      <c r="A19" s="144"/>
       <c r="B19" s="18" t="s">
         <v>29</v>
       </c>
@@ -13562,7 +13547,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="144"/>
+      <c r="A21" s="145"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -13642,7 +13627,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="144"/>
+      <c r="A23" s="145"/>
       <c r="B23" s="18" t="s">
         <v>29</v>
       </c>
@@ -13722,7 +13707,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="147"/>
+      <c r="A25" s="144"/>
       <c r="B25" s="18" t="s">
         <v>29</v>
       </c>
@@ -13802,7 +13787,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
+      <c r="A27" s="144"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -13882,7 +13867,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="147"/>
+      <c r="A29" s="144"/>
       <c r="B29" s="18" t="s">
         <v>29</v>
       </c>
@@ -13962,7 +13947,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="147"/>
+      <c r="A31" s="144"/>
       <c r="B31" s="18" t="s">
         <v>29</v>
       </c>
@@ -14002,6 +13987,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -14011,12 +14002,6 @@
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -14040,7 +14025,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -14059,7 +14044,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="145"/>
+      <c r="A2" s="146"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -14076,7 +14061,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="146"/>
+      <c r="A3" s="147"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -14134,7 +14119,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="144"/>
+      <c r="A5" s="145"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -14173,7 +14158,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="147"/>
+      <c r="A6" s="144"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -14253,7 +14238,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="144"/>
+      <c r="A8" s="145"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -14292,7 +14277,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
+      <c r="A9" s="144"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -14331,7 +14316,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="148" t="s">
+      <c r="A10" s="151" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -14372,7 +14357,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="149"/>
+      <c r="A11" s="152"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -14411,7 +14396,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
+      <c r="A12" s="152"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -14491,7 +14476,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="144"/>
+      <c r="A14" s="145"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -14530,7 +14515,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="147"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -14610,7 +14595,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="144"/>
+      <c r="A17" s="145"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -14649,7 +14634,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="147"/>
+      <c r="A18" s="144"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -14688,7 +14673,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="148" t="s">
+      <c r="A19" s="151" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -14729,7 +14714,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="149"/>
+      <c r="A20" s="152"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -14768,7 +14753,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="149"/>
+      <c r="A21" s="152"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -14848,7 +14833,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="144"/>
+      <c r="A23" s="145"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -14887,7 +14872,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="147"/>
+      <c r="A24" s="144"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -14967,7 +14952,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="144"/>
+      <c r="A26" s="145"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -15006,7 +14991,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
+      <c r="A27" s="144"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -15045,7 +15030,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="150"/>
+      <c r="A28" s="148"/>
       <c r="B28" s="16" t="s">
         <v>29</v>
       </c>
@@ -15084,7 +15069,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="151"/>
+      <c r="A29" s="149"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -15123,7 +15108,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="151"/>
+      <c r="A30" s="149"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -15162,7 +15147,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="150"/>
+      <c r="A31" s="148"/>
       <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
@@ -15201,7 +15186,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="151"/>
+      <c r="A32" s="149"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -15240,7 +15225,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="152"/>
+      <c r="A33" s="150"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -15279,7 +15264,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="150"/>
+      <c r="A34" s="148"/>
       <c r="B34" s="16" t="s">
         <v>29</v>
       </c>
@@ -15318,7 +15303,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="151"/>
+      <c r="A35" s="149"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -15357,7 +15342,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="152"/>
+      <c r="A36" s="150"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -15396,7 +15381,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="150"/>
+      <c r="A37" s="148"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
@@ -15435,7 +15420,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="151"/>
+      <c r="A38" s="149"/>
       <c r="B38" s="17" t="s">
         <v>29</v>
       </c>
@@ -15474,7 +15459,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="152"/>
+      <c r="A39" s="150"/>
       <c r="B39" s="18" t="s">
         <v>29</v>
       </c>
@@ -15514,6 +15499,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -15521,12 +15512,6 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -15644,7 +15629,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="144"/>
+      <c r="A5" s="145"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -15683,7 +15668,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="147"/>
+      <c r="A6" s="144"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -15763,7 +15748,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="144"/>
+      <c r="A8" s="145"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -15802,7 +15787,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
+      <c r="A9" s="144"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -15882,7 +15867,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="144"/>
+      <c r="A11" s="145"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -15921,7 +15906,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="144"/>
+      <c r="A12" s="145"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -16001,7 +15986,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="144"/>
+      <c r="A14" s="145"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -16040,7 +16025,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
+      <c r="A15" s="145"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -16120,7 +16105,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="144"/>
+      <c r="A17" s="145"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -16159,7 +16144,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
+      <c r="A18" s="145"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -16237,7 +16222,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="144"/>
+      <c r="A20" s="145"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -16276,7 +16261,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="144"/>
+      <c r="A21" s="145"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -16356,7 +16341,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="144"/>
+      <c r="A23" s="145"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -16395,7 +16380,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="147"/>
+      <c r="A24" s="144"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -16475,7 +16460,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="144"/>
+      <c r="A26" s="145"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -16514,7 +16499,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
+      <c r="A27" s="144"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -16594,7 +16579,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="144"/>
+      <c r="A29" s="145"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -16633,7 +16618,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="147"/>
+      <c r="A30" s="144"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -16713,7 +16698,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="144"/>
+      <c r="A32" s="145"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -16752,7 +16737,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="147"/>
+      <c r="A33" s="144"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -16832,7 +16817,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="144"/>
+      <c r="A35" s="145"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -16871,7 +16856,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="147"/>
+      <c r="A36" s="144"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -17000,7 +16985,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -17019,7 +17004,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="145"/>
+      <c r="A2" s="146"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -17036,7 +17021,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="146"/>
+      <c r="A3" s="147"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -17094,7 +17079,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="144"/>
+      <c r="A5" s="145"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -17133,7 +17118,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="147"/>
+      <c r="A6" s="144"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -17213,7 +17198,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="144"/>
+      <c r="A8" s="145"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -17252,7 +17237,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
+      <c r="A9" s="144"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -17332,7 +17317,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="144"/>
+      <c r="A11" s="145"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -17371,7 +17356,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="144"/>
+      <c r="A12" s="145"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -17451,7 +17436,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="144"/>
+      <c r="A14" s="145"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -17490,7 +17475,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
+      <c r="A15" s="145"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -17570,7 +17555,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="144"/>
+      <c r="A17" s="145"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -17609,7 +17594,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
+      <c r="A18" s="145"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -17648,7 +17633,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="150"/>
+      <c r="A19" s="148"/>
       <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
@@ -17687,7 +17672,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="151"/>
+      <c r="A20" s="149"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -17726,7 +17711,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="151"/>
+      <c r="A21" s="149"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -17806,7 +17791,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="144"/>
+      <c r="A23" s="145"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -17845,7 +17830,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="147"/>
+      <c r="A24" s="144"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -17925,7 +17910,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="144"/>
+      <c r="A26" s="145"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -17964,7 +17949,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
+      <c r="A27" s="144"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -18044,7 +18029,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="144"/>
+      <c r="A29" s="145"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -18083,7 +18068,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="144"/>
+      <c r="A30" s="145"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -18163,7 +18148,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="144"/>
+      <c r="A32" s="145"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -18202,7 +18187,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
+      <c r="A33" s="145"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -18282,7 +18267,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="144"/>
+      <c r="A35" s="145"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -18321,7 +18306,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="147"/>
+      <c r="A36" s="144"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -18360,7 +18345,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="145" t="s">
+      <c r="A37" s="146" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -18379,7 +18364,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="145"/>
+      <c r="A38" s="146"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
@@ -18396,7 +18381,7 @@
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="146"/>
+      <c r="A39" s="147"/>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -18414,6 +18399,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -18421,12 +18412,6 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -18450,7 +18435,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -18469,7 +18454,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="145"/>
+      <c r="A2" s="146"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -18486,7 +18471,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="146"/>
+      <c r="A3" s="147"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -18544,7 +18529,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="144"/>
+      <c r="A5" s="145"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -18583,7 +18568,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="147"/>
+      <c r="A6" s="144"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -18663,7 +18648,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="144"/>
+      <c r="A8" s="145"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -18702,7 +18687,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
+      <c r="A9" s="144"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -18782,7 +18767,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="144"/>
+      <c r="A11" s="145"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -18821,7 +18806,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="144"/>
+      <c r="A12" s="145"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -18901,7 +18886,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="144"/>
+      <c r="A14" s="145"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -18940,7 +18925,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
+      <c r="A15" s="145"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -19020,7 +19005,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="144"/>
+      <c r="A17" s="145"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -19059,7 +19044,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
+      <c r="A18" s="145"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -19139,7 +19124,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="144"/>
+      <c r="A20" s="145"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -19178,7 +19163,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="144"/>
+      <c r="A21" s="145"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -19258,7 +19243,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="144"/>
+      <c r="A23" s="145"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -19297,7 +19282,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="144"/>
+      <c r="A24" s="145"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -19377,7 +19362,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="144"/>
+      <c r="A26" s="145"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -19416,7 +19401,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
+      <c r="A27" s="144"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -19455,7 +19440,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="150"/>
+      <c r="A28" s="148"/>
       <c r="B28" s="16" t="s">
         <v>29</v>
       </c>
@@ -19494,7 +19479,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="151"/>
+      <c r="A29" s="149"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -19533,7 +19518,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="151"/>
+      <c r="A30" s="149"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -19572,7 +19557,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="150"/>
+      <c r="A31" s="148"/>
       <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
@@ -19611,7 +19596,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="151"/>
+      <c r="A32" s="149"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -19650,7 +19635,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="151"/>
+      <c r="A33" s="149"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -19689,7 +19674,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="150"/>
+      <c r="A34" s="148"/>
       <c r="B34" s="16" t="s">
         <v>29</v>
       </c>
@@ -19728,7 +19713,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="151"/>
+      <c r="A35" s="149"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -19767,7 +19752,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="152"/>
+      <c r="A36" s="150"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -19806,7 +19791,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="150"/>
+      <c r="A37" s="148"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
@@ -19845,7 +19830,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="151"/>
+      <c r="A38" s="149"/>
       <c r="B38" s="17" t="s">
         <v>29</v>
       </c>
@@ -19884,7 +19869,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="152"/>
+      <c r="A39" s="150"/>
       <c r="B39" s="18" t="s">
         <v>29</v>
       </c>
@@ -19924,6 +19909,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -19931,12 +19922,6 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -19960,7 +19945,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -19979,7 +19964,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="145"/>
+      <c r="A2" s="146"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -19996,7 +19981,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="146"/>
+      <c r="A3" s="147"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -20054,7 +20039,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="144"/>
+      <c r="A5" s="145"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -20093,7 +20078,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="147"/>
+      <c r="A6" s="144"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -20173,7 +20158,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="144"/>
+      <c r="A8" s="145"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -20212,7 +20197,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
+      <c r="A9" s="144"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -20292,7 +20277,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="144"/>
+      <c r="A11" s="145"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -20331,7 +20316,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="144"/>
+      <c r="A12" s="145"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -20411,7 +20396,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="144"/>
+      <c r="A14" s="145"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -20450,7 +20435,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
+      <c r="A15" s="145"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -20530,7 +20515,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="144"/>
+      <c r="A17" s="145"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -20569,7 +20554,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
+      <c r="A18" s="145"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -20608,7 +20593,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="150"/>
+      <c r="A19" s="148"/>
       <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
@@ -20647,7 +20632,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="151"/>
+      <c r="A20" s="149"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -20686,7 +20671,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="151"/>
+      <c r="A21" s="149"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -20766,7 +20751,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="144"/>
+      <c r="A23" s="145"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -20805,7 +20790,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="147"/>
+      <c r="A24" s="144"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -20885,7 +20870,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="144"/>
+      <c r="A26" s="145"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -20924,7 +20909,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
+      <c r="A27" s="144"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -21004,7 +20989,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="144"/>
+      <c r="A29" s="145"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -21043,7 +21028,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="144"/>
+      <c r="A30" s="145"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -21123,7 +21108,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="144"/>
+      <c r="A32" s="145"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -21162,7 +21147,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
+      <c r="A33" s="145"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -21242,7 +21227,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="144"/>
+      <c r="A35" s="145"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -21281,7 +21266,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
+      <c r="A36" s="145"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -21320,7 +21305,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="145" t="s">
+      <c r="A37" s="146" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -21339,7 +21324,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="145"/>
+      <c r="A38" s="146"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
@@ -21356,7 +21341,7 @@
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="146"/>
+      <c r="A39" s="147"/>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -21374,11 +21359,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A16:A18"/>
@@ -21387,6 +21367,11 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21415,7 +21400,7 @@
       <c r="B1" s="159" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="165"/>
+      <c r="C1" s="162"/>
       <c r="D1" s="159" t="s">
         <v>42</v>
       </c>
@@ -21423,19 +21408,19 @@
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="160"/>
-      <c r="C2" s="166"/>
+      <c r="C2" s="163"/>
       <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="160"/>
-      <c r="C3" s="166"/>
+      <c r="C3" s="163"/>
       <c r="D3" s="160"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="161"/>
-      <c r="C4" s="167"/>
+      <c r="C4" s="164"/>
       <c r="D4" s="161"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21443,7 +21428,7 @@
       <c r="B5" s="159" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="162"/>
+      <c r="C5" s="165"/>
       <c r="D5" s="159" t="s">
         <v>43</v>
       </c>
@@ -21451,19 +21436,19 @@
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="160"/>
-      <c r="C6" s="163"/>
+      <c r="C6" s="166"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="160"/>
-      <c r="C7" s="163"/>
+      <c r="C7" s="166"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="161"/>
-      <c r="C8" s="164"/>
+      <c r="C8" s="167"/>
       <c r="D8" s="161"/>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21471,7 +21456,7 @@
       <c r="B9" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="162"/>
+      <c r="C9" s="165"/>
       <c r="D9" s="159" t="s">
         <v>44</v>
       </c>
@@ -21479,19 +21464,19 @@
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="160"/>
-      <c r="C10" s="163"/>
+      <c r="C10" s="166"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="160"/>
-      <c r="C11" s="163"/>
+      <c r="C11" s="166"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="161"/>
-      <c r="C12" s="164"/>
+      <c r="C12" s="167"/>
       <c r="D12" s="161"/>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21499,7 +21484,7 @@
       <c r="B13" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="162"/>
+      <c r="C13" s="165"/>
       <c r="D13" s="159" t="s">
         <v>37</v>
       </c>
@@ -21507,19 +21492,19 @@
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="160"/>
-      <c r="C14" s="163"/>
+      <c r="C14" s="166"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="160"/>
-      <c r="C15" s="163"/>
+      <c r="C15" s="166"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="161"/>
-      <c r="C16" s="164"/>
+      <c r="C16" s="167"/>
       <c r="D16" s="161"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -21531,6 +21516,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -21539,14 +21532,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21576,7 +21561,7 @@
       <c r="B1" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="174"/>
+      <c r="C1" s="171"/>
       <c r="D1" s="159" t="s">
         <v>42</v>
       </c>
@@ -21584,19 +21569,19 @@
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="175"/>
+      <c r="C2" s="172"/>
       <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="175"/>
+      <c r="C3" s="172"/>
       <c r="D3" s="160"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="176"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="161"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21604,7 +21589,7 @@
       <c r="B5" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="171"/>
+      <c r="C5" s="174"/>
       <c r="D5" s="159" t="s">
         <v>43</v>
       </c>
@@ -21612,19 +21597,19 @@
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="172"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="172"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="173"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="161"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21632,7 +21617,7 @@
       <c r="B9" s="168" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="171"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="159" t="s">
         <v>44</v>
       </c>
@@ -21643,21 +21628,21 @@
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="172"/>
+      <c r="C10" s="175"/>
       <c r="D10" s="160"/>
       <c r="F10" s="160"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="172"/>
+      <c r="C11" s="175"/>
       <c r="D11" s="160"/>
       <c r="F11" s="160"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="173"/>
+      <c r="C12" s="176"/>
       <c r="D12" s="161"/>
       <c r="F12" s="161"/>
     </row>
@@ -21666,7 +21651,7 @@
       <c r="B13" s="168" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="171"/>
+      <c r="C13" s="174"/>
       <c r="D13" s="168" t="s">
         <v>37</v>
       </c>
@@ -21677,21 +21662,21 @@
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="172"/>
+      <c r="C14" s="175"/>
       <c r="D14" s="169"/>
       <c r="G14" s="160"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="172"/>
+      <c r="C15" s="175"/>
       <c r="D15" s="169"/>
       <c r="G15" s="160"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="173"/>
+      <c r="C16" s="176"/>
       <c r="D16" s="170"/>
       <c r="G16" s="161"/>
     </row>
@@ -21704,14 +21689,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
     <mergeCell ref="G13:G16"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
@@ -21722,6 +21699,14 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21751,27 +21736,27 @@
       <c r="B1" s="168" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="174"/>
+      <c r="C1" s="171"/>
       <c r="D1" s="168"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="175"/>
+      <c r="C2" s="172"/>
       <c r="D2" s="169"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="175"/>
+      <c r="C3" s="172"/>
       <c r="D3" s="169"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="176"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="170"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -21781,27 +21766,27 @@
       <c r="B5" s="168" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="171"/>
+      <c r="C5" s="174"/>
       <c r="D5" s="159"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="172"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="160"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="172"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="173"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="161"/>
       <c r="H8"/>
     </row>
@@ -21810,7 +21795,7 @@
       <c r="B9" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="171"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="159"/>
       <c r="G9"/>
       <c r="H9"/>
@@ -21818,48 +21803,56 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="172"/>
+      <c r="C10" s="175"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="172"/>
+      <c r="C11" s="175"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="173"/>
+      <c r="C12" s="176"/>
       <c r="D12" s="161"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="155"/>
       <c r="B13" s="168"/>
-      <c r="C13" s="171"/>
+      <c r="C13" s="174"/>
       <c r="D13" s="159"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="172"/>
+      <c r="C14" s="175"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="172"/>
+      <c r="C15" s="175"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="173"/>
+      <c r="C16" s="176"/>
       <c r="D16" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -21868,14 +21861,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22025,13 +22010,13 @@
       <c r="H8" s="49"/>
     </row>
     <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="94" t="s">
+      <c r="A11" s="108" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="94"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="108"/>
     </row>
     <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A12" s="65"/>
@@ -22041,165 +22026,156 @@
       <c r="E12" s="66"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="94" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="109" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="95"/>
-      <c r="B14" s="96" t="s">
+      <c r="A14" s="94"/>
+      <c r="B14" s="109" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
-      <c r="B15" s="96" t="s">
+      <c r="A15" s="94"/>
+      <c r="B15" s="109" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="95"/>
-      <c r="B16" s="96" t="s">
+      <c r="A16" s="94"/>
+      <c r="B16" s="109" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="109"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
-      <c r="B17" s="96" t="s">
+      <c r="A17" s="94"/>
+      <c r="B17" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="95" t="s">
+      <c r="A19" s="94" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="96" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="100"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="98"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="95"/>
-      <c r="B20" s="101"/>
-      <c r="C20" s="102"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="103"/>
+      <c r="A20" s="94"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="101"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="94" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="106"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="104"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="95"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="109"/>
+      <c r="A23" s="94"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="107"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="95"/>
-      <c r="B24" s="104" t="s">
+      <c r="A24" s="94"/>
+      <c r="B24" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="106"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="104"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="95"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="108"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="109"/>
+      <c r="A25" s="94"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="107"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="97" t="s">
+      <c r="B27" s="95" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="95"/>
-      <c r="B28" s="97"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="97"/>
-      <c r="E28" s="97"/>
+      <c r="A28" s="94"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="95"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
-      <c r="B29" s="97"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="97"/>
-      <c r="E29" s="97"/>
+      <c r="A29" s="94"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="95" t="s">
+      <c r="A31" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="97" t="s">
+      <c r="B31" s="95" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="97"/>
-      <c r="D31" s="97"/>
-      <c r="E31" s="97"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="95"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
-      <c r="B32" s="97"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
+      <c r="A32" s="94"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="95"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="95"/>
-      <c r="B33" s="97"/>
-      <c r="C33" s="97"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="97"/>
+      <c r="A33" s="94"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:E29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:E33"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:E20"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:E23"/>
-    <mergeCell ref="B24:E25"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B1:G1"/>
@@ -22210,6 +22186,15 @@
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:E29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:E33"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:E20"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:E23"/>
+    <mergeCell ref="B24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22238,7 +22223,7 @@
       <c r="B1" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="174"/>
+      <c r="C1" s="171"/>
       <c r="D1" s="168" t="s">
         <v>17</v>
       </c>
@@ -22246,20 +22231,20 @@
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="175"/>
+      <c r="C2" s="172"/>
       <c r="D2" s="169"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="175"/>
+      <c r="C3" s="172"/>
       <c r="D3" s="169"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="176"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="170"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -22269,7 +22254,7 @@
       <c r="B5" s="168" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="171"/>
+      <c r="C5" s="174"/>
       <c r="D5" s="159" t="s">
         <v>18</v>
       </c>
@@ -22278,19 +22263,19 @@
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="172"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="172"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="173"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="161"/>
       <c r="H8"/>
     </row>
@@ -22299,7 +22284,7 @@
       <c r="B9" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="171"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="159" t="s">
         <v>19</v>
       </c>
@@ -22309,19 +22294,19 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="172"/>
+      <c r="C10" s="175"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="172"/>
+      <c r="C11" s="175"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="173"/>
+      <c r="C12" s="176"/>
       <c r="D12" s="161"/>
       <c r="F12"/>
     </row>
@@ -22330,7 +22315,7 @@
       <c r="B13" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="171"/>
+      <c r="C13" s="174"/>
       <c r="D13" s="159" t="s">
         <v>20</v>
       </c>
@@ -22338,23 +22323,31 @@
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="172"/>
+      <c r="C14" s="175"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="172"/>
+      <c r="C15" s="175"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="173"/>
+      <c r="C16" s="176"/>
       <c r="D16" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -22363,14 +22356,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22400,7 +22385,7 @@
       <c r="B1" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="174"/>
+      <c r="C1" s="171"/>
       <c r="D1" s="159" t="s">
         <v>8</v>
       </c>
@@ -22408,19 +22393,19 @@
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="175"/>
+      <c r="C2" s="172"/>
       <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="175"/>
+      <c r="C3" s="172"/>
       <c r="D3" s="160"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="176"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="161"/>
       <c r="G4"/>
     </row>
@@ -22429,7 +22414,7 @@
       <c r="B5" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="171"/>
+      <c r="C5" s="174"/>
       <c r="D5" s="159" t="s">
         <v>7</v>
       </c>
@@ -22437,19 +22422,19 @@
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="172"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="172"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="173"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="161"/>
       <c r="H8"/>
     </row>
@@ -22458,7 +22443,7 @@
       <c r="B9" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="171"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="159" t="s">
         <v>9</v>
       </c>
@@ -22466,19 +22451,19 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="172"/>
+      <c r="C10" s="175"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="172"/>
+      <c r="C11" s="175"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="173"/>
+      <c r="C12" s="176"/>
       <c r="D12" s="161"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -22486,29 +22471,37 @@
       <c r="B13" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="171"/>
+      <c r="C13" s="174"/>
       <c r="D13" s="159"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="172"/>
+      <c r="C14" s="175"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="172"/>
+      <c r="C15" s="175"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="173"/>
+      <c r="C16" s="176"/>
       <c r="D16" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -22517,14 +22510,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22554,7 +22539,7 @@
       <c r="B1" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="174"/>
+      <c r="C1" s="171"/>
       <c r="D1" s="159" t="s">
         <v>31</v>
       </c>
@@ -22563,20 +22548,20 @@
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="175"/>
+      <c r="C2" s="172"/>
       <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="175"/>
+      <c r="C3" s="172"/>
       <c r="D3" s="160"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="176"/>
+      <c r="C4" s="173"/>
       <c r="D4" s="161"/>
       <c r="F4"/>
     </row>
@@ -22585,7 +22570,7 @@
       <c r="B5" s="168" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="171"/>
+      <c r="C5" s="174"/>
       <c r="D5" s="159" t="s">
         <v>34</v>
       </c>
@@ -22593,20 +22578,20 @@
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="172"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="172"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="160"/>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="173"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="161"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -22614,7 +22599,7 @@
       <c r="B9" s="168" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="171"/>
+      <c r="C9" s="174"/>
       <c r="D9" s="159" t="s">
         <v>35</v>
       </c>
@@ -22623,25 +22608,25 @@
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="172"/>
+      <c r="C10" s="175"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="172"/>
+      <c r="C11" s="175"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="173"/>
+      <c r="C12" s="176"/>
       <c r="D12" s="161"/>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="155"/>
       <c r="B13" s="168"/>
-      <c r="C13" s="171"/>
+      <c r="C13" s="174"/>
       <c r="D13" s="159" t="s">
         <v>36</v>
       </c>
@@ -22650,23 +22635,31 @@
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="172"/>
+      <c r="C14" s="175"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="172"/>
+      <c r="C15" s="175"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="173"/>
+      <c r="C16" s="176"/>
       <c r="D16" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -22675,14 +22668,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22835,14 +22820,14 @@
       <c r="F10" s="49"/>
     </row>
     <row r="12" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="108" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="94"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A13" s="65"/>
@@ -22853,180 +22838,173 @@
       <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="94" t="s">
         <v>162</v>
       </c>
       <c r="B14" s="70"/>
-      <c r="C14" s="96" t="s">
+      <c r="C14" s="109" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
+      <c r="A15" s="94"/>
       <c r="B15" s="70"/>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="109" t="s">
         <v>166</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="95"/>
+      <c r="A16" s="94"/>
       <c r="B16" s="70"/>
-      <c r="C16" s="96" t="s">
+      <c r="C16" s="109" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="109"/>
     </row>
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
+      <c r="A17" s="94"/>
       <c r="B17" s="70"/>
-      <c r="C17" s="96" t="s">
+      <c r="C17" s="109" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
     </row>
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="95"/>
+      <c r="A18" s="94"/>
       <c r="B18" s="70"/>
-      <c r="C18" s="96" t="s">
+      <c r="C18" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="95" t="s">
+      <c r="A20" s="94" t="s">
         <v>169</v>
       </c>
       <c r="B20" s="76"/>
-      <c r="C20" s="98" t="s">
+      <c r="C20" s="96" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="100"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="98"/>
     </row>
     <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
+      <c r="A21" s="94"/>
       <c r="B21" s="77"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="103"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="101"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="94" t="s">
         <v>171</v>
       </c>
       <c r="B23" s="76"/>
-      <c r="C23" s="104" t="s">
+      <c r="C23" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="106"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="104"/>
     </row>
     <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="95"/>
+      <c r="A24" s="94"/>
       <c r="B24" s="77"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="109"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="106"/>
+      <c r="F24" s="107"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="95"/>
+      <c r="A25" s="94"/>
       <c r="B25" s="76"/>
-      <c r="C25" s="104" t="s">
+      <c r="C25" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="106"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="104"/>
     </row>
     <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="95"/>
+      <c r="A26" s="94"/>
       <c r="B26" s="77"/>
-      <c r="C26" s="107"/>
-      <c r="D26" s="108"/>
-      <c r="E26" s="108"/>
-      <c r="F26" s="109"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="107"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="95" t="s">
+      <c r="A28" s="94" t="s">
         <v>174</v>
       </c>
       <c r="B28" s="70"/>
-      <c r="C28" s="97" t="s">
+      <c r="C28" s="95" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="97"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="97"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="95"/>
     </row>
     <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
+      <c r="A29" s="94"/>
       <c r="B29" s="70"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="97"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="97"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
     </row>
     <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="95"/>
+      <c r="A30" s="94"/>
       <c r="B30" s="70"/>
-      <c r="C30" s="97"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="97"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="95"/>
     </row>
     <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="95" t="s">
+      <c r="A32" s="94" t="s">
         <v>176</v>
       </c>
       <c r="B32" s="70"/>
-      <c r="C32" s="97" t="s">
+      <c r="C32" s="95" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="95"/>
     </row>
     <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="95"/>
+      <c r="A33" s="94"/>
       <c r="B33" s="70"/>
-      <c r="C33" s="97"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="97"/>
-      <c r="F33" s="97"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="95"/>
     </row>
     <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="95"/>
+      <c r="A34" s="94"/>
       <c r="B34" s="70"/>
-      <c r="C34" s="97"/>
-      <c r="D34" s="97"/>
-      <c r="E34" s="97"/>
-      <c r="F34" s="97"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C28:F30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C32:F34"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="C23:F24"/>
-    <mergeCell ref="C25:F26"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="C3:F3"/>
@@ -23038,6 +23016,13 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C28:F30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C32:F34"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="C23:F24"/>
+    <mergeCell ref="C25:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23501,6 +23486,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="A41:E41"/>
@@ -23509,12 +23500,6 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B27:E27"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23526,7 +23511,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -23549,31 +23534,31 @@
         <v>132</v>
       </c>
       <c r="E1" s="41">
-        <v>44725</v>
+        <v>44732</v>
       </c>
       <c r="F1" s="41">
         <f>E1+1</f>
-        <v>44726</v>
+        <v>44733</v>
       </c>
       <c r="G1" s="41">
         <f t="shared" ref="G1:K1" si="0">F1+1</f>
-        <v>44727</v>
+        <v>44734</v>
       </c>
       <c r="H1" s="41">
         <f t="shared" si="0"/>
-        <v>44728</v>
+        <v>44735</v>
       </c>
       <c r="I1" s="41">
         <f t="shared" si="0"/>
-        <v>44729</v>
+        <v>44736</v>
       </c>
       <c r="J1" s="41">
         <f t="shared" si="0"/>
-        <v>44730</v>
+        <v>44737</v>
       </c>
       <c r="K1" s="41">
         <f t="shared" si="0"/>
-        <v>44731</v>
+        <v>44738</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
@@ -23632,11 +23617,9 @@
       </c>
       <c r="D5" s="43">
         <f>SUM(E5:K5)</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="44">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E5" s="44"/>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
@@ -23669,11 +23652,13 @@
         <f>SUM(E7:K7)</f>
         <v>2</v>
       </c>
-      <c r="E7" s="44">
-        <v>2</v>
-      </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44">
+        <v>1</v>
+      </c>
+      <c r="G7" s="44">
+        <v>1</v>
+      </c>
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
       <c r="J7" s="44"/>
@@ -23744,10 +23729,15 @@
       <c r="C12" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="43"/>
+      <c r="D12" s="43">
+        <f>SUM(E12:K12)</f>
+        <v>1</v>
+      </c>
       <c r="E12" s="44"/>
       <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="G12" s="44">
+        <v>1</v>
+      </c>
       <c r="H12" s="44"/>
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
@@ -23760,9 +23750,14 @@
       <c r="C13" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="43"/>
+      <c r="D13" s="43">
+        <f>SUM(E13:K13)</f>
+        <v>1</v>
+      </c>
       <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
+      <c r="F13" s="44">
+        <v>1</v>
+      </c>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
       <c r="I13" s="44"/>
@@ -23774,10 +23769,7 @@
       <c r="C14" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="43">
-        <f>SUM(E14:K14)</f>
-        <v>0</v>
-      </c>
+      <c r="D14" s="43"/>
       <c r="E14" s="44"/>
       <c r="F14" s="44"/>
       <c r="G14" s="44"/>
@@ -23823,10 +23815,7 @@
       <c r="C17" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="43">
-        <f>SUM(E17:K17)</f>
-        <v>0</v>
-      </c>
+      <c r="D17" s="43"/>
       <c r="E17" s="44"/>
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
@@ -23854,10 +23843,7 @@
       <c r="C19" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="43">
-        <f>SUM(E19:K19)</f>
-        <v>0</v>
-      </c>
+      <c r="D19" s="43"/>
       <c r="E19" s="80"/>
       <c r="F19" s="80"/>
       <c r="G19" s="80"/>
@@ -23871,10 +23857,7 @@
       <c r="C20" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="43">
-        <f>SUM(E20:K20)</f>
-        <v>0</v>
-      </c>
+      <c r="D20" s="43"/>
       <c r="E20" s="80"/>
       <c r="F20" s="80"/>
       <c r="G20" s="80"/>
@@ -23891,10 +23874,7 @@
       <c r="C21" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="D21" s="43">
-        <f>SUM(E21:K21)</f>
-        <v>0</v>
-      </c>
+      <c r="D21" s="43"/>
       <c r="E21" s="44"/>
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
@@ -23906,15 +23886,15 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E22" s="7">
         <f t="shared" ref="E22:K22" si="1">SUM(E4:E21)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="1"/>
@@ -23941,44 +23921,39 @@
         <v>132</v>
       </c>
       <c r="E25" s="41">
-        <v>44725</v>
+        <v>44732</v>
       </c>
       <c r="F25" s="41">
         <f>E25+1</f>
-        <v>44726</v>
+        <v>44733</v>
       </c>
       <c r="G25" s="41">
         <f t="shared" ref="G25" si="2">F25+1</f>
-        <v>44727</v>
+        <v>44734</v>
       </c>
       <c r="H25" s="41">
         <f t="shared" ref="H25" si="3">G25+1</f>
-        <v>44728</v>
+        <v>44735</v>
       </c>
       <c r="I25" s="41">
         <f t="shared" ref="I25" si="4">H25+1</f>
-        <v>44729</v>
+        <v>44736</v>
       </c>
       <c r="J25" s="41">
         <f t="shared" ref="J25" si="5">I25+1</f>
-        <v>44730</v>
+        <v>44737</v>
       </c>
       <c r="K25" s="41">
         <f t="shared" ref="K25" si="6">J25+1</f>
-        <v>44731</v>
+        <v>44738</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C26" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="D26" s="43">
-        <f>SUM(E26:K26)</f>
-        <v>1</v>
-      </c>
-      <c r="E26" s="84">
-        <v>1</v>
-      </c>
+      <c r="D26" s="43"/>
+      <c r="E26" s="84"/>
       <c r="F26" s="84"/>
       <c r="G26" s="84"/>
       <c r="H26" s="84"/>
@@ -23990,13 +23965,8 @@
       <c r="C27" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="D27" s="43">
-        <f>SUM(E27:K27)</f>
-        <v>1</v>
-      </c>
-      <c r="E27" s="84">
-        <v>1</v>
-      </c>
+      <c r="D27" s="43"/>
+      <c r="E27" s="84"/>
       <c r="F27" s="84"/>
       <c r="G27" s="84"/>
       <c r="H27" s="84"/>

</xml_diff>

<commit_message>
Lenovo Ideapad 320, Checkin Timestamp :: Wed 07/06/2022-14:23:06.54;
</commit_message>
<xml_diff>
--- a/My Transformation Journey.xlsx
+++ b/My Transformation Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nc\Awakening-The-Giant-Naresh-Chaurasia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DE45CF-4DC6-4FD7-B998-0398644F8AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502BA6A0-A8B7-4910-8DB3-3296B3E52B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="4" xr2:uid="{45287DFE-D99B-4274-A6CA-7DF7915FBBA5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Soft Skills" sheetId="46" r:id="rId2"/>
     <sheet name="Job Sheet" sheetId="45" r:id="rId3"/>
     <sheet name="Goal Sheet" sheetId="38" r:id="rId4"/>
-    <sheet name="Week 12.06" sheetId="43" r:id="rId5"/>
+    <sheet name="Week 27.06" sheetId="43" r:id="rId5"/>
     <sheet name="Week 21.05" sheetId="41" r:id="rId6"/>
     <sheet name="Sheet5" sheetId="42" r:id="rId7"/>
     <sheet name="Dashboard" sheetId="39" r:id="rId8"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2841" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="200">
   <si>
     <t>Legs</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>Double Up</t>
+  </si>
+  <si>
+    <t>Salsa</t>
   </si>
 </sst>
 </file>
@@ -2126,7 +2129,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Week 12.06'!$D$1</c:f>
+              <c:f>'Week 27.06'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2207,7 +2210,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Week 12.06'!$C$4:$C$21</c:f>
+              <c:f>'Week 27.06'!$C$4:$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -2269,21 +2272,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Week 12.06'!$D$4:$D$21</c:f>
+              <c:f>'Week 27.06'!$D$4:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2580,48 +2601,48 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Week 12.06'!$E$1:$K$1</c:f>
+              <c:f>'Week 27.06'!$E$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>dd\ mmm</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44732</c:v>
+                  <c:v>44746</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44733</c:v>
+                  <c:v>44747</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44734</c:v>
+                  <c:v>44748</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44735</c:v>
+                  <c:v>44749</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44736</c:v>
+                  <c:v>44750</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44737</c:v>
+                  <c:v>44751</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44738</c:v>
+                  <c:v>44752</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Week 12.06'!$E$22:$K$22</c:f>
+              <c:f>'Week 27.06'!$E$22:$K$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2874,24 +2895,30 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Week 12.06'!$C$26:$C$31</c:f>
+              <c:f>'Week 27.06'!$C$26:$C$31</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Shuffle-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Double Up</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>Salsa</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Week 12.06'!$D$26:$D$31</c:f>
+              <c:f>'Week 27.06'!$D$26:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11519,7 +11546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A659E6A-7EE0-4249-A963-0689D0721EB6}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -21872,7 +21899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE5C14C-9149-426E-99EC-FCF3B5351889}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B17" sqref="B17:E17"/>
     </sheetView>
   </sheetViews>
@@ -23511,7 +23538,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -23534,31 +23561,31 @@
         <v>132</v>
       </c>
       <c r="E1" s="41">
-        <v>44732</v>
+        <v>44746</v>
       </c>
       <c r="F1" s="41">
         <f>E1+1</f>
-        <v>44733</v>
+        <v>44747</v>
       </c>
       <c r="G1" s="41">
         <f t="shared" ref="G1:K1" si="0">F1+1</f>
-        <v>44734</v>
+        <v>44748</v>
       </c>
       <c r="H1" s="41">
         <f t="shared" si="0"/>
-        <v>44735</v>
+        <v>44749</v>
       </c>
       <c r="I1" s="41">
         <f t="shared" si="0"/>
-        <v>44736</v>
+        <v>44750</v>
       </c>
       <c r="J1" s="41">
         <f t="shared" si="0"/>
-        <v>44737</v>
+        <v>44751</v>
       </c>
       <c r="K1" s="41">
         <f t="shared" si="0"/>
-        <v>44738</v>
+        <v>44752</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
@@ -23617,9 +23644,11 @@
       </c>
       <c r="D5" s="43">
         <f>SUM(E5:K5)</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="44"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="44">
+        <v>1</v>
+      </c>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
@@ -23632,7 +23661,10 @@
       <c r="C6" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="43"/>
+      <c r="D6" s="43">
+        <f>SUM(E6:K6)</f>
+        <v>0</v>
+      </c>
       <c r="E6" s="44"/>
       <c r="F6" s="44"/>
       <c r="G6" s="44"/>
@@ -23650,15 +23682,11 @@
       </c>
       <c r="D7" s="43">
         <f>SUM(E7:K7)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" s="44"/>
-      <c r="F7" s="44">
-        <v>1</v>
-      </c>
-      <c r="G7" s="44">
-        <v>1</v>
-      </c>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
       <c r="J7" s="44"/>
@@ -23671,7 +23699,10 @@
       <c r="C8" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="43"/>
+      <c r="D8" s="43">
+        <f>SUM(E8:K8)</f>
+        <v>0</v>
+      </c>
       <c r="E8" s="44"/>
       <c r="F8" s="44"/>
       <c r="G8" s="44"/>
@@ -23685,7 +23716,10 @@
       <c r="C9" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="43">
+        <f>SUM(E9:K9)</f>
+        <v>0</v>
+      </c>
       <c r="E9" s="44"/>
       <c r="F9" s="44"/>
       <c r="G9" s="44"/>
@@ -23731,13 +23765,11 @@
       </c>
       <c r="D12" s="43">
         <f>SUM(E12:K12)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="44"/>
       <c r="F12" s="44"/>
-      <c r="G12" s="44">
-        <v>1</v>
-      </c>
+      <c r="G12" s="44"/>
       <c r="H12" s="44"/>
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
@@ -23752,12 +23784,10 @@
       </c>
       <c r="D13" s="43">
         <f>SUM(E13:K13)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="44"/>
-      <c r="F13" s="44">
-        <v>1</v>
-      </c>
+      <c r="F13" s="44"/>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
       <c r="I13" s="44"/>
@@ -23815,9 +23845,14 @@
       <c r="C17" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="43"/>
+      <c r="D17" s="43">
+        <f>SUM(E17:K17)</f>
+        <v>1</v>
+      </c>
       <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
+      <c r="F17" s="44">
+        <v>1</v>
+      </c>
       <c r="G17" s="44"/>
       <c r="H17" s="44"/>
       <c r="I17" s="44"/>
@@ -23829,8 +23864,13 @@
       <c r="C18" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="80"/>
+      <c r="D18" s="43">
+        <f>SUM(E18:K18)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="80">
+        <v>1</v>
+      </c>
       <c r="F18" s="80"/>
       <c r="G18" s="80"/>
       <c r="H18" s="80"/>
@@ -23874,7 +23914,10 @@
       <c r="C21" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="D21" s="43"/>
+      <c r="D21" s="43">
+        <f>SUM(E21:K21)</f>
+        <v>0</v>
+      </c>
       <c r="E21" s="44"/>
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
@@ -23886,15 +23929,15 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E22" s="7">
         <f t="shared" ref="E22:K22" si="1">SUM(E4:E21)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="1"/>
@@ -23921,31 +23964,31 @@
         <v>132</v>
       </c>
       <c r="E25" s="41">
-        <v>44732</v>
+        <v>44739</v>
       </c>
       <c r="F25" s="41">
         <f>E25+1</f>
-        <v>44733</v>
+        <v>44740</v>
       </c>
       <c r="G25" s="41">
         <f t="shared" ref="G25" si="2">F25+1</f>
-        <v>44734</v>
+        <v>44741</v>
       </c>
       <c r="H25" s="41">
         <f t="shared" ref="H25" si="3">G25+1</f>
-        <v>44735</v>
+        <v>44742</v>
       </c>
       <c r="I25" s="41">
         <f t="shared" ref="I25" si="4">H25+1</f>
-        <v>44736</v>
+        <v>44743</v>
       </c>
       <c r="J25" s="41">
         <f t="shared" ref="J25" si="5">I25+1</f>
-        <v>44737</v>
+        <v>44744</v>
       </c>
       <c r="K25" s="41">
         <f t="shared" ref="K25" si="6">J25+1</f>
-        <v>44738</v>
+        <v>44745</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -23975,8 +24018,13 @@
       <c r="K27" s="84"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C28" s="45"/>
-      <c r="D28" s="43"/>
+      <c r="C28" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="D28" s="43">
+        <f>SUM(E28:K28)</f>
+        <v>0</v>
+      </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="84"/>

</xml_diff>

<commit_message>
Lenovo Ideapad 320, Checkin Timestamp :: Thu 07/07/2022-14:17:16.17;
</commit_message>
<xml_diff>
--- a/My Transformation Journey.xlsx
+++ b/My Transformation Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nc\Awakening-The-Giant-Naresh-Chaurasia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502BA6A0-A8B7-4910-8DB3-3296B3E52B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D3CACA-B0A1-4D14-B80E-09CE2711FB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="4" xr2:uid="{45287DFE-D99B-4274-A6CA-7DF7915FBBA5}"/>
   </bookViews>
@@ -1774,8 +1774,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1815,12 +1821,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1924,9 +1924,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1936,6 +1933,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1943,12 +1949,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1979,6 +1979,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1986,15 +1995,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2006,6 +2006,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2013,15 +2022,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2277,13 +2277,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2301,7 +2301,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -2642,10 +2642,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -12840,7 +12840,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="145" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -12859,7 +12859,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="146"/>
+      <c r="A2" s="145"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -12876,7 +12876,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="147"/>
+      <c r="A3" s="146"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -12934,7 +12934,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="144"/>
+      <c r="A5" s="147"/>
       <c r="B5" s="18" t="s">
         <v>29</v>
       </c>
@@ -13014,7 +13014,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="144"/>
+      <c r="A7" s="147"/>
       <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
@@ -13094,7 +13094,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="145"/>
+      <c r="A9" s="144"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -13174,7 +13174,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="145"/>
+      <c r="A11" s="144"/>
       <c r="B11" s="18" t="s">
         <v>29</v>
       </c>
@@ -13254,7 +13254,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="145"/>
+      <c r="A13" s="144"/>
       <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
@@ -13334,7 +13334,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="145"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -13414,7 +13414,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="145"/>
+      <c r="A17" s="144"/>
       <c r="B17" s="18" t="s">
         <v>29</v>
       </c>
@@ -13494,7 +13494,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="144"/>
+      <c r="A19" s="147"/>
       <c r="B19" s="18" t="s">
         <v>29</v>
       </c>
@@ -13574,7 +13574,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="145"/>
+      <c r="A21" s="144"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -13654,7 +13654,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="145"/>
+      <c r="A23" s="144"/>
       <c r="B23" s="18" t="s">
         <v>29</v>
       </c>
@@ -13734,7 +13734,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="144"/>
+      <c r="A25" s="147"/>
       <c r="B25" s="18" t="s">
         <v>29</v>
       </c>
@@ -13814,7 +13814,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
+      <c r="A27" s="147"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -13894,7 +13894,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="144"/>
+      <c r="A29" s="147"/>
       <c r="B29" s="18" t="s">
         <v>29</v>
       </c>
@@ -13974,7 +13974,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="144"/>
+      <c r="A31" s="147"/>
       <c r="B31" s="18" t="s">
         <v>29</v>
       </c>
@@ -14014,12 +14014,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -14029,6 +14023,12 @@
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -14052,7 +14052,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="145" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -14071,7 +14071,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="146"/>
+      <c r="A2" s="145"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -14088,7 +14088,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="147"/>
+      <c r="A3" s="146"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -14146,7 +14146,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="145"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -14185,7 +14185,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="144"/>
+      <c r="A6" s="147"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -14265,7 +14265,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="145"/>
+      <c r="A8" s="144"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -14304,7 +14304,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="144"/>
+      <c r="A9" s="147"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -14343,7 +14343,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="151" t="s">
+      <c r="A10" s="148" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -14384,7 +14384,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="152"/>
+      <c r="A11" s="149"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -14423,7 +14423,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="152"/>
+      <c r="A12" s="149"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -14503,7 +14503,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="145"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -14542,7 +14542,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
+      <c r="A15" s="147"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -14622,7 +14622,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="145"/>
+      <c r="A17" s="144"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -14661,7 +14661,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
+      <c r="A18" s="147"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -14700,7 +14700,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="151" t="s">
+      <c r="A19" s="148" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -14741,7 +14741,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="152"/>
+      <c r="A20" s="149"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -14780,7 +14780,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="152"/>
+      <c r="A21" s="149"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -14860,7 +14860,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="145"/>
+      <c r="A23" s="144"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -14899,7 +14899,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="144"/>
+      <c r="A24" s="147"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -14979,7 +14979,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="145"/>
+      <c r="A26" s="144"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -15018,7 +15018,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
+      <c r="A27" s="147"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -15057,7 +15057,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="148"/>
+      <c r="A28" s="150"/>
       <c r="B28" s="16" t="s">
         <v>29</v>
       </c>
@@ -15096,7 +15096,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="149"/>
+      <c r="A29" s="151"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -15135,7 +15135,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="149"/>
+      <c r="A30" s="151"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -15174,7 +15174,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="148"/>
+      <c r="A31" s="150"/>
       <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
@@ -15213,7 +15213,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="149"/>
+      <c r="A32" s="151"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -15252,7 +15252,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="150"/>
+      <c r="A33" s="152"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -15291,7 +15291,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="148"/>
+      <c r="A34" s="150"/>
       <c r="B34" s="16" t="s">
         <v>29</v>
       </c>
@@ -15330,7 +15330,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="149"/>
+      <c r="A35" s="151"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -15369,7 +15369,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="150"/>
+      <c r="A36" s="152"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -15408,7 +15408,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="148"/>
+      <c r="A37" s="150"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
@@ -15447,7 +15447,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="149"/>
+      <c r="A38" s="151"/>
       <c r="B38" s="17" t="s">
         <v>29</v>
       </c>
@@ -15486,7 +15486,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="150"/>
+      <c r="A39" s="152"/>
       <c r="B39" s="18" t="s">
         <v>29</v>
       </c>
@@ -15526,12 +15526,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -15539,6 +15533,12 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -15656,7 +15656,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="145"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -15695,7 +15695,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="144"/>
+      <c r="A6" s="147"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -15775,7 +15775,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="145"/>
+      <c r="A8" s="144"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -15814,7 +15814,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="144"/>
+      <c r="A9" s="147"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -15894,7 +15894,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="145"/>
+      <c r="A11" s="144"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -15933,7 +15933,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="145"/>
+      <c r="A12" s="144"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -16013,7 +16013,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="145"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -16052,7 +16052,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="145"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -16132,7 +16132,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="145"/>
+      <c r="A17" s="144"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -16171,7 +16171,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="145"/>
+      <c r="A18" s="144"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -16249,7 +16249,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="145"/>
+      <c r="A20" s="144"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -16288,7 +16288,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="145"/>
+      <c r="A21" s="144"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -16368,7 +16368,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="145"/>
+      <c r="A23" s="144"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -16407,7 +16407,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="144"/>
+      <c r="A24" s="147"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -16487,7 +16487,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="145"/>
+      <c r="A26" s="144"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -16526,7 +16526,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
+      <c r="A27" s="147"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -16606,7 +16606,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="145"/>
+      <c r="A29" s="144"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -16645,7 +16645,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="144"/>
+      <c r="A30" s="147"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -16725,7 +16725,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="145"/>
+      <c r="A32" s="144"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -16764,7 +16764,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
+      <c r="A33" s="147"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -16844,7 +16844,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="145"/>
+      <c r="A35" s="144"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -16883,7 +16883,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
+      <c r="A36" s="147"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -17012,7 +17012,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="145" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -17031,7 +17031,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="146"/>
+      <c r="A2" s="145"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -17048,7 +17048,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="147"/>
+      <c r="A3" s="146"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -17106,7 +17106,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="145"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -17145,7 +17145,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="144"/>
+      <c r="A6" s="147"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -17225,7 +17225,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="145"/>
+      <c r="A8" s="144"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -17264,7 +17264,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="144"/>
+      <c r="A9" s="147"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -17344,7 +17344,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="145"/>
+      <c r="A11" s="144"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -17383,7 +17383,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="145"/>
+      <c r="A12" s="144"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -17463,7 +17463,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="145"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -17502,7 +17502,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="145"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -17582,7 +17582,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="145"/>
+      <c r="A17" s="144"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -17621,7 +17621,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="145"/>
+      <c r="A18" s="144"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -17660,7 +17660,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="148"/>
+      <c r="A19" s="150"/>
       <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
@@ -17699,7 +17699,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="149"/>
+      <c r="A20" s="151"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -17738,7 +17738,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="149"/>
+      <c r="A21" s="151"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -17818,7 +17818,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="145"/>
+      <c r="A23" s="144"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -17857,7 +17857,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="144"/>
+      <c r="A24" s="147"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -17937,7 +17937,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="145"/>
+      <c r="A26" s="144"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -17976,7 +17976,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
+      <c r="A27" s="147"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -18056,7 +18056,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="145"/>
+      <c r="A29" s="144"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -18095,7 +18095,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="145"/>
+      <c r="A30" s="144"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -18175,7 +18175,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="145"/>
+      <c r="A32" s="144"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -18214,7 +18214,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="145"/>
+      <c r="A33" s="144"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -18294,7 +18294,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="145"/>
+      <c r="A35" s="144"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -18333,7 +18333,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
+      <c r="A36" s="147"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -18372,7 +18372,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="146" t="s">
+      <c r="A37" s="145" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -18391,7 +18391,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="146"/>
+      <c r="A38" s="145"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
@@ -18408,7 +18408,7 @@
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="147"/>
+      <c r="A39" s="146"/>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -18426,12 +18426,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -18439,6 +18433,12 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -18462,7 +18462,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="145" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -18481,7 +18481,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="146"/>
+      <c r="A2" s="145"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -18498,7 +18498,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="147"/>
+      <c r="A3" s="146"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -18556,7 +18556,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="145"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -18595,7 +18595,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="144"/>
+      <c r="A6" s="147"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -18675,7 +18675,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="145"/>
+      <c r="A8" s="144"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -18714,7 +18714,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="144"/>
+      <c r="A9" s="147"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -18794,7 +18794,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="145"/>
+      <c r="A11" s="144"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -18833,7 +18833,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="145"/>
+      <c r="A12" s="144"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -18913,7 +18913,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="145"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -18952,7 +18952,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="145"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -19032,7 +19032,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="145"/>
+      <c r="A17" s="144"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -19071,7 +19071,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="145"/>
+      <c r="A18" s="144"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -19151,7 +19151,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="145"/>
+      <c r="A20" s="144"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -19190,7 +19190,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="145"/>
+      <c r="A21" s="144"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -19270,7 +19270,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="145"/>
+      <c r="A23" s="144"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -19309,7 +19309,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="145"/>
+      <c r="A24" s="144"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -19389,7 +19389,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="145"/>
+      <c r="A26" s="144"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -19428,7 +19428,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
+      <c r="A27" s="147"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -19467,7 +19467,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="148"/>
+      <c r="A28" s="150"/>
       <c r="B28" s="16" t="s">
         <v>29</v>
       </c>
@@ -19506,7 +19506,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="149"/>
+      <c r="A29" s="151"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -19545,7 +19545,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="149"/>
+      <c r="A30" s="151"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -19584,7 +19584,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="148"/>
+      <c r="A31" s="150"/>
       <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
@@ -19623,7 +19623,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="149"/>
+      <c r="A32" s="151"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -19662,7 +19662,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="149"/>
+      <c r="A33" s="151"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -19701,7 +19701,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="148"/>
+      <c r="A34" s="150"/>
       <c r="B34" s="16" t="s">
         <v>29</v>
       </c>
@@ -19740,7 +19740,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="149"/>
+      <c r="A35" s="151"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -19779,7 +19779,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="150"/>
+      <c r="A36" s="152"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -19818,7 +19818,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="148"/>
+      <c r="A37" s="150"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
@@ -19857,7 +19857,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="149"/>
+      <c r="A38" s="151"/>
       <c r="B38" s="17" t="s">
         <v>29</v>
       </c>
@@ -19896,7 +19896,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="150"/>
+      <c r="A39" s="152"/>
       <c r="B39" s="18" t="s">
         <v>29</v>
       </c>
@@ -19936,12 +19936,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -19949,6 +19943,12 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -19972,7 +19972,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="145" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -19991,7 +19991,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="146"/>
+      <c r="A2" s="145"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -20008,7 +20008,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="147"/>
+      <c r="A3" s="146"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -20066,7 +20066,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="145"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -20105,7 +20105,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="144"/>
+      <c r="A6" s="147"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -20185,7 +20185,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="145"/>
+      <c r="A8" s="144"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -20224,7 +20224,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="144"/>
+      <c r="A9" s="147"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -20304,7 +20304,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="145"/>
+      <c r="A11" s="144"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -20343,7 +20343,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="145"/>
+      <c r="A12" s="144"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -20423,7 +20423,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="145"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -20462,7 +20462,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="145"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -20542,7 +20542,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="145"/>
+      <c r="A17" s="144"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -20581,7 +20581,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="145"/>
+      <c r="A18" s="144"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -20620,7 +20620,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="148"/>
+      <c r="A19" s="150"/>
       <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
@@ -20659,7 +20659,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="149"/>
+      <c r="A20" s="151"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -20698,7 +20698,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="149"/>
+      <c r="A21" s="151"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -20778,7 +20778,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="145"/>
+      <c r="A23" s="144"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -20817,7 +20817,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="144"/>
+      <c r="A24" s="147"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -20897,7 +20897,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="145"/>
+      <c r="A26" s="144"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -20936,7 +20936,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
+      <c r="A27" s="147"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -21016,7 +21016,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="145"/>
+      <c r="A29" s="144"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -21055,7 +21055,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="145"/>
+      <c r="A30" s="144"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -21135,7 +21135,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="145"/>
+      <c r="A32" s="144"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -21174,7 +21174,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="145"/>
+      <c r="A33" s="144"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -21254,7 +21254,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="145"/>
+      <c r="A35" s="144"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -21293,7 +21293,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="145"/>
+      <c r="A36" s="144"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -21332,7 +21332,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="146" t="s">
+      <c r="A37" s="145" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -21351,7 +21351,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="146"/>
+      <c r="A38" s="145"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
@@ -21368,7 +21368,7 @@
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="147"/>
+      <c r="A39" s="146"/>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -21386,6 +21386,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A16:A18"/>
@@ -21394,11 +21399,6 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21427,7 +21427,7 @@
       <c r="B1" s="159" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="162"/>
+      <c r="C1" s="165"/>
       <c r="D1" s="159" t="s">
         <v>42</v>
       </c>
@@ -21435,19 +21435,19 @@
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="160"/>
-      <c r="C2" s="163"/>
+      <c r="C2" s="166"/>
       <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="160"/>
-      <c r="C3" s="163"/>
+      <c r="C3" s="166"/>
       <c r="D3" s="160"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="161"/>
-      <c r="C4" s="164"/>
+      <c r="C4" s="167"/>
       <c r="D4" s="161"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21455,7 +21455,7 @@
       <c r="B5" s="159" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="165"/>
+      <c r="C5" s="162"/>
       <c r="D5" s="159" t="s">
         <v>43</v>
       </c>
@@ -21463,19 +21463,19 @@
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="160"/>
-      <c r="C6" s="166"/>
+      <c r="C6" s="163"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="160"/>
-      <c r="C7" s="166"/>
+      <c r="C7" s="163"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="161"/>
-      <c r="C8" s="167"/>
+      <c r="C8" s="164"/>
       <c r="D8" s="161"/>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21483,7 +21483,7 @@
       <c r="B9" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="165"/>
+      <c r="C9" s="162"/>
       <c r="D9" s="159" t="s">
         <v>44</v>
       </c>
@@ -21491,19 +21491,19 @@
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="160"/>
-      <c r="C10" s="166"/>
+      <c r="C10" s="163"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="160"/>
-      <c r="C11" s="166"/>
+      <c r="C11" s="163"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="161"/>
-      <c r="C12" s="167"/>
+      <c r="C12" s="164"/>
       <c r="D12" s="161"/>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21511,7 +21511,7 @@
       <c r="B13" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="165"/>
+      <c r="C13" s="162"/>
       <c r="D13" s="159" t="s">
         <v>37</v>
       </c>
@@ -21519,19 +21519,19 @@
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="160"/>
-      <c r="C14" s="166"/>
+      <c r="C14" s="163"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="160"/>
-      <c r="C15" s="166"/>
+      <c r="C15" s="163"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="161"/>
-      <c r="C16" s="167"/>
+      <c r="C16" s="164"/>
       <c r="D16" s="161"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -21543,6 +21543,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -21551,14 +21559,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21588,7 +21588,7 @@
       <c r="B1" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="171"/>
+      <c r="C1" s="174"/>
       <c r="D1" s="159" t="s">
         <v>42</v>
       </c>
@@ -21596,19 +21596,19 @@
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="172"/>
+      <c r="C2" s="175"/>
       <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="172"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="160"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="173"/>
+      <c r="C4" s="176"/>
       <c r="D4" s="161"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21616,7 +21616,7 @@
       <c r="B5" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="174"/>
+      <c r="C5" s="171"/>
       <c r="D5" s="159" t="s">
         <v>43</v>
       </c>
@@ -21624,19 +21624,19 @@
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="175"/>
+      <c r="C6" s="172"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="175"/>
+      <c r="C7" s="172"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="176"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="161"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21644,7 +21644,7 @@
       <c r="B9" s="168" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="174"/>
+      <c r="C9" s="171"/>
       <c r="D9" s="159" t="s">
         <v>44</v>
       </c>
@@ -21655,21 +21655,21 @@
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="175"/>
+      <c r="C10" s="172"/>
       <c r="D10" s="160"/>
       <c r="F10" s="160"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="175"/>
+      <c r="C11" s="172"/>
       <c r="D11" s="160"/>
       <c r="F11" s="160"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="176"/>
+      <c r="C12" s="173"/>
       <c r="D12" s="161"/>
       <c r="F12" s="161"/>
     </row>
@@ -21678,7 +21678,7 @@
       <c r="B13" s="168" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="174"/>
+      <c r="C13" s="171"/>
       <c r="D13" s="168" t="s">
         <v>37</v>
       </c>
@@ -21689,21 +21689,21 @@
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="175"/>
+      <c r="C14" s="172"/>
       <c r="D14" s="169"/>
       <c r="G14" s="160"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="175"/>
+      <c r="C15" s="172"/>
       <c r="D15" s="169"/>
       <c r="G15" s="160"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="176"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="170"/>
       <c r="G16" s="161"/>
     </row>
@@ -21716,6 +21716,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="G13:G16"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
@@ -21726,14 +21734,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21763,27 +21763,27 @@
       <c r="B1" s="168" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="171"/>
+      <c r="C1" s="174"/>
       <c r="D1" s="168"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="172"/>
+      <c r="C2" s="175"/>
       <c r="D2" s="169"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="172"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="169"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="173"/>
+      <c r="C4" s="176"/>
       <c r="D4" s="170"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -21793,27 +21793,27 @@
       <c r="B5" s="168" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="174"/>
+      <c r="C5" s="171"/>
       <c r="D5" s="159"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="175"/>
+      <c r="C6" s="172"/>
       <c r="D6" s="160"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="175"/>
+      <c r="C7" s="172"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="176"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="161"/>
       <c r="H8"/>
     </row>
@@ -21822,7 +21822,7 @@
       <c r="B9" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="174"/>
+      <c r="C9" s="171"/>
       <c r="D9" s="159"/>
       <c r="G9"/>
       <c r="H9"/>
@@ -21830,48 +21830,56 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="175"/>
+      <c r="C10" s="172"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="175"/>
+      <c r="C11" s="172"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="176"/>
+      <c r="C12" s="173"/>
       <c r="D12" s="161"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="155"/>
       <c r="B13" s="168"/>
-      <c r="C13" s="174"/>
+      <c r="C13" s="171"/>
       <c r="D13" s="159"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="175"/>
+      <c r="C14" s="172"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="175"/>
+      <c r="C15" s="172"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="176"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -21880,14 +21888,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22037,13 +22037,13 @@
       <c r="H8" s="49"/>
     </row>
     <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="108" t="s">
+      <c r="A11" s="94" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="108"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
     </row>
     <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A12" s="65"/>
@@ -22053,156 +22053,165 @@
       <c r="E12" s="66"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="95" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="96" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="94"/>
-      <c r="B14" s="109" t="s">
+      <c r="A14" s="95"/>
+      <c r="B14" s="96" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="94"/>
-      <c r="B15" s="109" t="s">
+      <c r="A15" s="95"/>
+      <c r="B15" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="94"/>
-      <c r="B16" s="109" t="s">
+      <c r="A16" s="95"/>
+      <c r="B16" s="96" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="94"/>
-      <c r="B17" s="109" t="s">
+      <c r="A17" s="95"/>
+      <c r="B17" s="96" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="94" t="s">
+      <c r="A19" s="95" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="98" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
-      <c r="E19" s="98"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
+      <c r="E19" s="100"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="94"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="101"/>
+      <c r="A20" s="95"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="103"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="95" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="104"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="106"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="94"/>
-      <c r="B23" s="105"/>
-      <c r="C23" s="106"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="107"/>
+      <c r="A23" s="95"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="109"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="94"/>
-      <c r="B24" s="102" t="s">
+      <c r="A24" s="95"/>
+      <c r="B24" s="104" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="104"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="106"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="94"/>
-      <c r="B25" s="105"/>
-      <c r="C25" s="106"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="107"/>
+      <c r="A25" s="95"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="108"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="109"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="95" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="95" t="s">
+      <c r="B27" s="97" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="94"/>
-      <c r="B28" s="95"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="95"/>
-      <c r="E28" s="95"/>
+      <c r="A28" s="95"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="97"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="94"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
+      <c r="A29" s="95"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="97"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="94" t="s">
+      <c r="A31" s="95" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="97" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="97"/>
+      <c r="E31" s="97"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="94"/>
-      <c r="B32" s="95"/>
-      <c r="C32" s="95"/>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
+      <c r="A32" s="95"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
-      <c r="B33" s="95"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
+      <c r="A33" s="95"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:E29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:E33"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:E20"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:E23"/>
+    <mergeCell ref="B24:E25"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B1:G1"/>
@@ -22213,15 +22222,6 @@
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:E29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:E33"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:E20"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:E23"/>
-    <mergeCell ref="B24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22250,7 +22250,7 @@
       <c r="B1" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="171"/>
+      <c r="C1" s="174"/>
       <c r="D1" s="168" t="s">
         <v>17</v>
       </c>
@@ -22258,20 +22258,20 @@
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="172"/>
+      <c r="C2" s="175"/>
       <c r="D2" s="169"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="172"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="169"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="173"/>
+      <c r="C4" s="176"/>
       <c r="D4" s="170"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -22281,7 +22281,7 @@
       <c r="B5" s="168" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="174"/>
+      <c r="C5" s="171"/>
       <c r="D5" s="159" t="s">
         <v>18</v>
       </c>
@@ -22290,19 +22290,19 @@
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="175"/>
+      <c r="C6" s="172"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="175"/>
+      <c r="C7" s="172"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="176"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="161"/>
       <c r="H8"/>
     </row>
@@ -22311,7 +22311,7 @@
       <c r="B9" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="174"/>
+      <c r="C9" s="171"/>
       <c r="D9" s="159" t="s">
         <v>19</v>
       </c>
@@ -22321,19 +22321,19 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="175"/>
+      <c r="C10" s="172"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="175"/>
+      <c r="C11" s="172"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="176"/>
+      <c r="C12" s="173"/>
       <c r="D12" s="161"/>
       <c r="F12"/>
     </row>
@@ -22342,7 +22342,7 @@
       <c r="B13" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="174"/>
+      <c r="C13" s="171"/>
       <c r="D13" s="159" t="s">
         <v>20</v>
       </c>
@@ -22350,23 +22350,31 @@
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="175"/>
+      <c r="C14" s="172"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="175"/>
+      <c r="C15" s="172"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="176"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -22375,14 +22383,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22412,7 +22412,7 @@
       <c r="B1" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="171"/>
+      <c r="C1" s="174"/>
       <c r="D1" s="159" t="s">
         <v>8</v>
       </c>
@@ -22420,19 +22420,19 @@
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="172"/>
+      <c r="C2" s="175"/>
       <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="172"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="160"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="173"/>
+      <c r="C4" s="176"/>
       <c r="D4" s="161"/>
       <c r="G4"/>
     </row>
@@ -22441,7 +22441,7 @@
       <c r="B5" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="174"/>
+      <c r="C5" s="171"/>
       <c r="D5" s="159" t="s">
         <v>7</v>
       </c>
@@ -22449,19 +22449,19 @@
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="175"/>
+      <c r="C6" s="172"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="175"/>
+      <c r="C7" s="172"/>
       <c r="D7" s="160"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="176"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="161"/>
       <c r="H8"/>
     </row>
@@ -22470,7 +22470,7 @@
       <c r="B9" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="174"/>
+      <c r="C9" s="171"/>
       <c r="D9" s="159" t="s">
         <v>9</v>
       </c>
@@ -22478,19 +22478,19 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="175"/>
+      <c r="C10" s="172"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="175"/>
+      <c r="C11" s="172"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="176"/>
+      <c r="C12" s="173"/>
       <c r="D12" s="161"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -22498,29 +22498,37 @@
       <c r="B13" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="174"/>
+      <c r="C13" s="171"/>
       <c r="D13" s="159"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="175"/>
+      <c r="C14" s="172"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="175"/>
+      <c r="C15" s="172"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="176"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -22529,14 +22537,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22566,7 +22566,7 @@
       <c r="B1" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="171"/>
+      <c r="C1" s="174"/>
       <c r="D1" s="159" t="s">
         <v>31</v>
       </c>
@@ -22575,20 +22575,20 @@
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="156"/>
       <c r="B2" s="169"/>
-      <c r="C2" s="172"/>
+      <c r="C2" s="175"/>
       <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="157"/>
       <c r="B3" s="169"/>
-      <c r="C3" s="172"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="160"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="158"/>
       <c r="B4" s="170"/>
-      <c r="C4" s="173"/>
+      <c r="C4" s="176"/>
       <c r="D4" s="161"/>
       <c r="F4"/>
     </row>
@@ -22597,7 +22597,7 @@
       <c r="B5" s="168" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="174"/>
+      <c r="C5" s="171"/>
       <c r="D5" s="159" t="s">
         <v>34</v>
       </c>
@@ -22605,20 +22605,20 @@
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="156"/>
       <c r="B6" s="169"/>
-      <c r="C6" s="175"/>
+      <c r="C6" s="172"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="169"/>
-      <c r="C7" s="175"/>
+      <c r="C7" s="172"/>
       <c r="D7" s="160"/>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="158"/>
       <c r="B8" s="170"/>
-      <c r="C8" s="176"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="161"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -22626,7 +22626,7 @@
       <c r="B9" s="168" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="174"/>
+      <c r="C9" s="171"/>
       <c r="D9" s="159" t="s">
         <v>35</v>
       </c>
@@ -22635,25 +22635,25 @@
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="156"/>
       <c r="B10" s="169"/>
-      <c r="C10" s="175"/>
+      <c r="C10" s="172"/>
       <c r="D10" s="160"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="157"/>
       <c r="B11" s="169"/>
-      <c r="C11" s="175"/>
+      <c r="C11" s="172"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="158"/>
       <c r="B12" s="170"/>
-      <c r="C12" s="176"/>
+      <c r="C12" s="173"/>
       <c r="D12" s="161"/>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="155"/>
       <c r="B13" s="168"/>
-      <c r="C13" s="174"/>
+      <c r="C13" s="171"/>
       <c r="D13" s="159" t="s">
         <v>36</v>
       </c>
@@ -22662,23 +22662,31 @@
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="156"/>
       <c r="B14" s="169"/>
-      <c r="C14" s="175"/>
+      <c r="C14" s="172"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="157"/>
       <c r="B15" s="169"/>
-      <c r="C15" s="175"/>
+      <c r="C15" s="172"/>
       <c r="D15" s="160"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="158"/>
       <c r="B16" s="170"/>
-      <c r="C16" s="176"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -22687,14 +22695,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22847,14 +22847,14 @@
       <c r="F10" s="49"/>
     </row>
     <row r="12" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="108" t="s">
+      <c r="A12" s="94" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="108"/>
-      <c r="C12" s="108"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
     </row>
     <row r="13" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A13" s="65"/>
@@ -22865,173 +22865,180 @@
       <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="95" t="s">
         <v>162</v>
       </c>
       <c r="B14" s="70"/>
-      <c r="C14" s="109" t="s">
+      <c r="C14" s="96" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="94"/>
+      <c r="A15" s="95"/>
       <c r="B15" s="70"/>
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="96" t="s">
         <v>166</v>
       </c>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="94"/>
+      <c r="A16" s="95"/>
       <c r="B16" s="70"/>
-      <c r="C16" s="109" t="s">
+      <c r="C16" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
     </row>
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="94"/>
+      <c r="A17" s="95"/>
       <c r="B17" s="70"/>
-      <c r="C17" s="109" t="s">
+      <c r="C17" s="96" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
     </row>
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
+      <c r="A18" s="95"/>
       <c r="B18" s="70"/>
-      <c r="C18" s="109" t="s">
+      <c r="C18" s="96" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="94" t="s">
+      <c r="A20" s="95" t="s">
         <v>169</v>
       </c>
       <c r="B20" s="76"/>
-      <c r="C20" s="96" t="s">
+      <c r="C20" s="98" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="97"/>
-      <c r="E20" s="97"/>
-      <c r="F20" s="98"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="100"/>
     </row>
     <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="94"/>
+      <c r="A21" s="95"/>
       <c r="B21" s="77"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="101"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="103"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="95" t="s">
         <v>171</v>
       </c>
       <c r="B23" s="76"/>
-      <c r="C23" s="102" t="s">
+      <c r="C23" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="104"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="106"/>
     </row>
     <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="94"/>
+      <c r="A24" s="95"/>
       <c r="B24" s="77"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="106"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="107"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="109"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="94"/>
+      <c r="A25" s="95"/>
       <c r="B25" s="76"/>
-      <c r="C25" s="102" t="s">
+      <c r="C25" s="104" t="s">
         <v>173</v>
       </c>
-      <c r="D25" s="103"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="104"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="106"/>
     </row>
     <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="94"/>
+      <c r="A26" s="95"/>
       <c r="B26" s="77"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="107"/>
+      <c r="C26" s="107"/>
+      <c r="D26" s="108"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="109"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="94" t="s">
+      <c r="A28" s="95" t="s">
         <v>174</v>
       </c>
       <c r="B28" s="70"/>
-      <c r="C28" s="95" t="s">
+      <c r="C28" s="97" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="95"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="95"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
     </row>
     <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="94"/>
+      <c r="A29" s="95"/>
       <c r="B29" s="70"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="95"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="97"/>
     </row>
     <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="94"/>
+      <c r="A30" s="95"/>
       <c r="B30" s="70"/>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="97"/>
     </row>
     <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="95" t="s">
         <v>176</v>
       </c>
       <c r="B32" s="70"/>
-      <c r="C32" s="95" t="s">
+      <c r="C32" s="97" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="95"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
     </row>
     <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
+      <c r="A33" s="95"/>
       <c r="B33" s="70"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="95"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
     </row>
     <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="94"/>
+      <c r="A34" s="95"/>
       <c r="B34" s="70"/>
-      <c r="C34" s="95"/>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C28:F30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C32:F34"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="C23:F24"/>
+    <mergeCell ref="C25:F26"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="C3:F3"/>
@@ -23043,13 +23050,6 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C28:F30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C32:F34"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="C23:F24"/>
-    <mergeCell ref="C25:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23513,12 +23513,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B13:E13"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="A41:E41"/>
@@ -23527,6 +23521,12 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B27:E27"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23538,7 +23538,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -23644,13 +23644,15 @@
       </c>
       <c r="D5" s="43">
         <f>SUM(E5:K5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="44">
         <v>1</v>
       </c>
       <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
+      <c r="G5" s="44">
+        <v>1</v>
+      </c>
       <c r="H5" s="44"/>
       <c r="I5" s="44"/>
       <c r="J5" s="44"/>
@@ -23663,11 +23665,13 @@
       </c>
       <c r="D6" s="43">
         <f>SUM(E6:K6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="44"/>
       <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
+      <c r="G6" s="44">
+        <v>1</v>
+      </c>
       <c r="H6" s="44"/>
       <c r="I6" s="44"/>
       <c r="J6" s="44"/>
@@ -23682,12 +23686,14 @@
       </c>
       <c r="D7" s="43">
         <f>SUM(E7:K7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="44"/>
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
+      <c r="H7" s="44">
+        <v>1</v>
+      </c>
       <c r="I7" s="44"/>
       <c r="J7" s="44"/>
       <c r="K7" s="44"/>
@@ -23866,13 +23872,15 @@
       </c>
       <c r="D18" s="43">
         <f>SUM(E18:K18)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="80">
         <v>1</v>
       </c>
       <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
+      <c r="G18" s="80">
+        <v>1</v>
+      </c>
       <c r="H18" s="80"/>
       <c r="I18" s="80"/>
       <c r="J18" s="80"/>
@@ -23937,11 +23945,11 @@
       </c>
       <c r="G22" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="7">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Lenovo Ideapad 320, Checkin Timestamp :: Fri 07/15/2022-17:43:19.24;
</commit_message>
<xml_diff>
--- a/My Transformation Journey.xlsx
+++ b/My Transformation Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nc\Awakening-The-Giant-Naresh-Chaurasia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6E5A30-FE3E-4181-BF81-1BFDE1A87FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A4F08-765F-474A-8265-CDE941728090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="5" xr2:uid="{45287DFE-D99B-4274-A6CA-7DF7915FBBA5}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Soft Skills" sheetId="46" r:id="rId3"/>
     <sheet name="Job Sheet" sheetId="45" r:id="rId4"/>
     <sheet name="Goal Sheet" sheetId="38" r:id="rId5"/>
-    <sheet name="Week 10.07.22" sheetId="43" r:id="rId6"/>
+    <sheet name="July 10.07.22" sheetId="43" r:id="rId6"/>
     <sheet name="Week 21.05" sheetId="41" r:id="rId7"/>
     <sheet name="Sheet5" sheetId="42" r:id="rId8"/>
     <sheet name="Dashboard" sheetId="39" r:id="rId9"/>
@@ -1775,6 +1775,12 @@
     <xf numFmtId="1" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1786,12 +1792,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1820,8 +1820,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1861,12 +1867,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1970,9 +1970,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1982,6 +1979,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1989,12 +1995,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2025,6 +2025,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2032,15 +2041,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2052,6 +2052,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2059,15 +2068,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2175,7 +2175,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Week 10.07.22'!$D$1</c:f>
+              <c:f>'July 10.07.22'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2256,7 +2256,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Week 10.07.22'!$C$4:$C$21</c:f>
+              <c:f>'July 10.07.22'!$C$4:$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -2318,18 +2318,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Week 10.07.22'!$D$4:$D$21</c:f>
+              <c:f>'July 10.07.22'!$D$4:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2341,7 +2341,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2356,7 +2356,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2653,7 +2653,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Week 10.07.22'!$E$1:$K$1</c:f>
+              <c:f>'July 10.07.22'!$E$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>dd\ mmm</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2683,7 +2683,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Week 10.07.22'!$E$22:$K$22</c:f>
+              <c:f>'July 10.07.22'!$E$22:$K$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2700,10 +2700,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2947,7 +2947,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Week 10.07.22'!$C$26:$C$31</c:f>
+              <c:f>'July 10.07.22'!$C$26:$C$31</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2964,7 +2964,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Week 10.07.22'!$D$26:$D$31</c:f>
+              <c:f>'July 10.07.22'!$D$26:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11612,10 +11612,10 @@
       <c r="A1" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="92" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="91"/>
+      <c r="C1" s="93"/>
       <c r="D1" s="89">
         <v>5</v>
       </c>
@@ -11658,10 +11658,10 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="88"/>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="94" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="93"/>
+      <c r="C2" s="95"/>
       <c r="D2" s="89"/>
       <c r="E2" s="89"/>
       <c r="F2" s="89"/>
@@ -11677,8 +11677,8 @@
       <c r="A3" s="87">
         <v>44753</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="91"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="85"/>
@@ -11695,8 +11695,8 @@
         <f>A3+1</f>
         <v>44754</v>
       </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="95"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="91"/>
       <c r="D4" s="85"/>
       <c r="E4" s="85"/>
       <c r="F4" s="85"/>
@@ -11713,8 +11713,8 @@
         <f t="shared" ref="A5:A23" si="1">A4+1</f>
         <v>44755</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="91"/>
       <c r="D5" s="85"/>
       <c r="E5" s="85"/>
       <c r="F5" s="85"/>
@@ -11731,8 +11731,8 @@
         <f t="shared" si="1"/>
         <v>44756</v>
       </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="91"/>
       <c r="D6" s="85"/>
       <c r="E6" s="85"/>
       <c r="F6" s="85"/>
@@ -11749,8 +11749,8 @@
         <f t="shared" si="1"/>
         <v>44757</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="95"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="85"/>
       <c r="E7" s="85"/>
       <c r="F7" s="85"/>
@@ -11767,8 +11767,8 @@
         <f t="shared" si="1"/>
         <v>44758</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="95"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="85"/>
       <c r="E8" s="85"/>
       <c r="F8" s="85"/>
@@ -11785,8 +11785,8 @@
         <f t="shared" si="1"/>
         <v>44759</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="95"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="91"/>
       <c r="D9" s="85"/>
       <c r="E9" s="85"/>
       <c r="F9" s="85"/>
@@ -11803,8 +11803,8 @@
         <f t="shared" si="1"/>
         <v>44760</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="95"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="85"/>
       <c r="E10" s="85"/>
       <c r="F10" s="85"/>
@@ -11821,8 +11821,8 @@
         <f t="shared" si="1"/>
         <v>44761</v>
       </c>
-      <c r="B11" s="94"/>
-      <c r="C11" s="95"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="85"/>
       <c r="E11" s="85"/>
       <c r="F11" s="85"/>
@@ -11839,8 +11839,8 @@
         <f t="shared" si="1"/>
         <v>44762</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="95"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="85"/>
       <c r="E12" s="85"/>
       <c r="F12" s="85"/>
@@ -11857,8 +11857,8 @@
         <f t="shared" si="1"/>
         <v>44763</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="95"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="85"/>
       <c r="E13" s="85"/>
       <c r="F13" s="85"/>
@@ -11875,8 +11875,8 @@
         <f t="shared" si="1"/>
         <v>44764</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="95"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="91"/>
       <c r="D14" s="85"/>
       <c r="E14" s="85"/>
       <c r="F14" s="85"/>
@@ -11893,8 +11893,8 @@
         <f t="shared" si="1"/>
         <v>44765</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="95"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="91"/>
       <c r="D15" s="85"/>
       <c r="E15" s="85"/>
       <c r="F15" s="85"/>
@@ -11911,8 +11911,8 @@
         <f t="shared" si="1"/>
         <v>44766</v>
       </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="95"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="91"/>
       <c r="D16" s="85"/>
       <c r="E16" s="85"/>
       <c r="F16" s="85"/>
@@ -11929,8 +11929,8 @@
         <f t="shared" si="1"/>
         <v>44767</v>
       </c>
-      <c r="B17" s="94"/>
-      <c r="C17" s="95"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="91"/>
       <c r="D17" s="85"/>
       <c r="E17" s="85"/>
       <c r="F17" s="85"/>
@@ -11947,8 +11947,8 @@
         <f t="shared" si="1"/>
         <v>44768</v>
       </c>
-      <c r="B18" s="94"/>
-      <c r="C18" s="95"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="91"/>
       <c r="D18" s="85"/>
       <c r="E18" s="85"/>
       <c r="F18" s="85"/>
@@ -11965,8 +11965,8 @@
         <f t="shared" si="1"/>
         <v>44769</v>
       </c>
-      <c r="B19" s="94"/>
-      <c r="C19" s="95"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="91"/>
       <c r="D19" s="85"/>
       <c r="E19" s="85"/>
       <c r="F19" s="85"/>
@@ -11983,8 +11983,8 @@
         <f>A19+1</f>
         <v>44770</v>
       </c>
-      <c r="B20" s="94"/>
-      <c r="C20" s="95"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="91"/>
       <c r="D20" s="85"/>
       <c r="E20" s="85"/>
       <c r="F20" s="85"/>
@@ -12001,8 +12001,8 @@
         <f t="shared" si="1"/>
         <v>44771</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="95"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="91"/>
       <c r="D21" s="85"/>
       <c r="E21" s="85"/>
       <c r="F21" s="85"/>
@@ -12019,8 +12019,8 @@
         <f t="shared" si="1"/>
         <v>44772</v>
       </c>
-      <c r="B22" s="94"/>
-      <c r="C22" s="95"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="91"/>
       <c r="D22" s="85"/>
       <c r="E22" s="85"/>
       <c r="F22" s="85"/>
@@ -12037,8 +12037,8 @@
         <f t="shared" si="1"/>
         <v>44773</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="95"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="91"/>
       <c r="D23" s="85"/>
       <c r="E23" s="85"/>
       <c r="F23" s="85"/>
@@ -12052,13 +12052,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B21:C21"/>
@@ -12075,6 +12068,13 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12924,7 +12924,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -12943,7 +12943,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="157"/>
+      <c r="A2" s="156"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -12960,7 +12960,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="158"/>
+      <c r="A3" s="157"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -13018,7 +13018,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="155"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="18" t="s">
         <v>29</v>
       </c>
@@ -13098,7 +13098,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="155"/>
+      <c r="A7" s="158"/>
       <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
@@ -13178,7 +13178,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="156"/>
+      <c r="A9" s="155"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -13258,7 +13258,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="156"/>
+      <c r="A11" s="155"/>
       <c r="B11" s="18" t="s">
         <v>29</v>
       </c>
@@ -13338,7 +13338,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="156"/>
+      <c r="A13" s="155"/>
       <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
@@ -13418,7 +13418,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="156"/>
+      <c r="A15" s="155"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -13498,7 +13498,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="156"/>
+      <c r="A17" s="155"/>
       <c r="B17" s="18" t="s">
         <v>29</v>
       </c>
@@ -13578,7 +13578,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="155"/>
+      <c r="A19" s="158"/>
       <c r="B19" s="18" t="s">
         <v>29</v>
       </c>
@@ -13658,7 +13658,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="156"/>
+      <c r="A21" s="155"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -13738,7 +13738,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="156"/>
+      <c r="A23" s="155"/>
       <c r="B23" s="18" t="s">
         <v>29</v>
       </c>
@@ -13818,7 +13818,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="155"/>
+      <c r="A25" s="158"/>
       <c r="B25" s="18" t="s">
         <v>29</v>
       </c>
@@ -13898,7 +13898,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
+      <c r="A27" s="158"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -13978,7 +13978,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="155"/>
+      <c r="A29" s="158"/>
       <c r="B29" s="18" t="s">
         <v>29</v>
       </c>
@@ -14058,7 +14058,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="155"/>
+      <c r="A31" s="158"/>
       <c r="B31" s="18" t="s">
         <v>29</v>
       </c>
@@ -14098,12 +14098,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -14113,6 +14107,12 @@
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -14136,7 +14136,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -14155,7 +14155,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="157"/>
+      <c r="A2" s="156"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -14172,7 +14172,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="158"/>
+      <c r="A3" s="157"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -14230,7 +14230,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="156"/>
+      <c r="A5" s="155"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -14269,7 +14269,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
+      <c r="A6" s="158"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -14349,7 +14349,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="156"/>
+      <c r="A8" s="155"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -14388,7 +14388,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
+      <c r="A9" s="158"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -14427,7 +14427,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="162" t="s">
+      <c r="A10" s="159" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -14468,7 +14468,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="163"/>
+      <c r="A11" s="160"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -14507,7 +14507,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="163"/>
+      <c r="A12" s="160"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -14587,7 +14587,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="156"/>
+      <c r="A14" s="155"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -14626,7 +14626,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="155"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -14706,7 +14706,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="156"/>
+      <c r="A17" s="155"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -14745,7 +14745,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="155"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -14784,7 +14784,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="162" t="s">
+      <c r="A19" s="159" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -14825,7 +14825,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="163"/>
+      <c r="A20" s="160"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -14864,7 +14864,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="163"/>
+      <c r="A21" s="160"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -14944,7 +14944,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="156"/>
+      <c r="A23" s="155"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -14983,7 +14983,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
+      <c r="A24" s="158"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -15063,7 +15063,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="156"/>
+      <c r="A26" s="155"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -15102,7 +15102,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
+      <c r="A27" s="158"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -15141,7 +15141,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="159"/>
+      <c r="A28" s="161"/>
       <c r="B28" s="16" t="s">
         <v>29</v>
       </c>
@@ -15180,7 +15180,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="160"/>
+      <c r="A29" s="162"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -15219,7 +15219,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="160"/>
+      <c r="A30" s="162"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -15258,7 +15258,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="159"/>
+      <c r="A31" s="161"/>
       <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
@@ -15297,7 +15297,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="160"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -15336,7 +15336,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="161"/>
+      <c r="A33" s="163"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -15375,7 +15375,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="159"/>
+      <c r="A34" s="161"/>
       <c r="B34" s="16" t="s">
         <v>29</v>
       </c>
@@ -15414,7 +15414,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="160"/>
+      <c r="A35" s="162"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -15453,7 +15453,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="161"/>
+      <c r="A36" s="163"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -15492,7 +15492,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="159"/>
+      <c r="A37" s="161"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
@@ -15531,7 +15531,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="160"/>
+      <c r="A38" s="162"/>
       <c r="B38" s="17" t="s">
         <v>29</v>
       </c>
@@ -15570,7 +15570,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="161"/>
+      <c r="A39" s="163"/>
       <c r="B39" s="18" t="s">
         <v>29</v>
       </c>
@@ -15610,12 +15610,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -15623,6 +15617,12 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -15740,7 +15740,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="156"/>
+      <c r="A5" s="155"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -15779,7 +15779,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
+      <c r="A6" s="158"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -15859,7 +15859,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="156"/>
+      <c r="A8" s="155"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -15898,7 +15898,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
+      <c r="A9" s="158"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -15978,7 +15978,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="156"/>
+      <c r="A11" s="155"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -16017,7 +16017,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="156"/>
+      <c r="A12" s="155"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -16097,7 +16097,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="156"/>
+      <c r="A14" s="155"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -16136,7 +16136,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="156"/>
+      <c r="A15" s="155"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -16216,7 +16216,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="156"/>
+      <c r="A17" s="155"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -16255,7 +16255,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="156"/>
+      <c r="A18" s="155"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -16333,7 +16333,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="156"/>
+      <c r="A20" s="155"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -16372,7 +16372,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="156"/>
+      <c r="A21" s="155"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -16452,7 +16452,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="156"/>
+      <c r="A23" s="155"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -16491,7 +16491,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
+      <c r="A24" s="158"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -16571,7 +16571,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="156"/>
+      <c r="A26" s="155"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -16610,7 +16610,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
+      <c r="A27" s="158"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -16690,7 +16690,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="156"/>
+      <c r="A29" s="155"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -16729,7 +16729,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="155"/>
+      <c r="A30" s="158"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -16809,7 +16809,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="156"/>
+      <c r="A32" s="155"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -16848,7 +16848,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="155"/>
+      <c r="A33" s="158"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -16928,7 +16928,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="156"/>
+      <c r="A35" s="155"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -16967,7 +16967,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="155"/>
+      <c r="A36" s="158"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -17096,7 +17096,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -17115,7 +17115,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="157"/>
+      <c r="A2" s="156"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -17132,7 +17132,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="158"/>
+      <c r="A3" s="157"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -17190,7 +17190,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="156"/>
+      <c r="A5" s="155"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -17229,7 +17229,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
+      <c r="A6" s="158"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -17309,7 +17309,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="156"/>
+      <c r="A8" s="155"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -17348,7 +17348,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
+      <c r="A9" s="158"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -17428,7 +17428,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="156"/>
+      <c r="A11" s="155"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -17467,7 +17467,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="156"/>
+      <c r="A12" s="155"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -17547,7 +17547,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="156"/>
+      <c r="A14" s="155"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -17586,7 +17586,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="156"/>
+      <c r="A15" s="155"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -17666,7 +17666,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="156"/>
+      <c r="A17" s="155"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -17705,7 +17705,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="156"/>
+      <c r="A18" s="155"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -17744,7 +17744,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="159"/>
+      <c r="A19" s="161"/>
       <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
@@ -17783,7 +17783,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="160"/>
+      <c r="A20" s="162"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -17822,7 +17822,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="160"/>
+      <c r="A21" s="162"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -17902,7 +17902,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="156"/>
+      <c r="A23" s="155"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -17941,7 +17941,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
+      <c r="A24" s="158"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -18021,7 +18021,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="156"/>
+      <c r="A26" s="155"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -18060,7 +18060,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
+      <c r="A27" s="158"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -18140,7 +18140,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="156"/>
+      <c r="A29" s="155"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -18179,7 +18179,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="156"/>
+      <c r="A30" s="155"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -18259,7 +18259,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="156"/>
+      <c r="A32" s="155"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -18298,7 +18298,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="156"/>
+      <c r="A33" s="155"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -18378,7 +18378,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="156"/>
+      <c r="A35" s="155"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -18417,7 +18417,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="155"/>
+      <c r="A36" s="158"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -18456,7 +18456,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="157" t="s">
+      <c r="A37" s="156" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -18475,7 +18475,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="157"/>
+      <c r="A38" s="156"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
@@ -18492,7 +18492,7 @@
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="158"/>
+      <c r="A39" s="157"/>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -18510,12 +18510,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -18523,6 +18517,12 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -18546,7 +18546,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -18565,7 +18565,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="157"/>
+      <c r="A2" s="156"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -18582,7 +18582,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="158"/>
+      <c r="A3" s="157"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -18640,7 +18640,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="156"/>
+      <c r="A5" s="155"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -18679,7 +18679,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
+      <c r="A6" s="158"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -18759,7 +18759,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="156"/>
+      <c r="A8" s="155"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -18798,7 +18798,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
+      <c r="A9" s="158"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -18878,7 +18878,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="156"/>
+      <c r="A11" s="155"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -18917,7 +18917,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="156"/>
+      <c r="A12" s="155"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -18997,7 +18997,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="156"/>
+      <c r="A14" s="155"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -19036,7 +19036,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="156"/>
+      <c r="A15" s="155"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -19116,7 +19116,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="156"/>
+      <c r="A17" s="155"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -19155,7 +19155,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="156"/>
+      <c r="A18" s="155"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -19235,7 +19235,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="156"/>
+      <c r="A20" s="155"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -19274,7 +19274,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="156"/>
+      <c r="A21" s="155"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -19354,7 +19354,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="156"/>
+      <c r="A23" s="155"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -19393,7 +19393,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="156"/>
+      <c r="A24" s="155"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -19473,7 +19473,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="156"/>
+      <c r="A26" s="155"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -19512,7 +19512,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
+      <c r="A27" s="158"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -19551,7 +19551,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="159"/>
+      <c r="A28" s="161"/>
       <c r="B28" s="16" t="s">
         <v>29</v>
       </c>
@@ -19590,7 +19590,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="160"/>
+      <c r="A29" s="162"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -19629,7 +19629,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="160"/>
+      <c r="A30" s="162"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -19668,7 +19668,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="159"/>
+      <c r="A31" s="161"/>
       <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
@@ -19707,7 +19707,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="160"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -19746,7 +19746,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="160"/>
+      <c r="A33" s="162"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -19785,7 +19785,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="159"/>
+      <c r="A34" s="161"/>
       <c r="B34" s="16" t="s">
         <v>29</v>
       </c>
@@ -19824,7 +19824,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="160"/>
+      <c r="A35" s="162"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -19863,7 +19863,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="161"/>
+      <c r="A36" s="163"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -19902,7 +19902,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="159"/>
+      <c r="A37" s="161"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
@@ -19941,7 +19941,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="160"/>
+      <c r="A38" s="162"/>
       <c r="B38" s="17" t="s">
         <v>29</v>
       </c>
@@ -19980,7 +19980,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="161"/>
+      <c r="A39" s="163"/>
       <c r="B39" s="18" t="s">
         <v>29</v>
       </c>
@@ -20020,12 +20020,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -20033,6 +20027,12 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -20056,7 +20056,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -20075,7 +20075,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="157"/>
+      <c r="A2" s="156"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -20092,7 +20092,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="158"/>
+      <c r="A3" s="157"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -20150,7 +20150,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="156"/>
+      <c r="A5" s="155"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -20189,7 +20189,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
+      <c r="A6" s="158"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -20269,7 +20269,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="156"/>
+      <c r="A8" s="155"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -20308,7 +20308,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
+      <c r="A9" s="158"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -20388,7 +20388,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="156"/>
+      <c r="A11" s="155"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -20427,7 +20427,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="156"/>
+      <c r="A12" s="155"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -20507,7 +20507,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="156"/>
+      <c r="A14" s="155"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -20546,7 +20546,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="156"/>
+      <c r="A15" s="155"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -20626,7 +20626,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="156"/>
+      <c r="A17" s="155"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -20665,7 +20665,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="156"/>
+      <c r="A18" s="155"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -20704,7 +20704,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="159"/>
+      <c r="A19" s="161"/>
       <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
@@ -20743,7 +20743,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="160"/>
+      <c r="A20" s="162"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -20782,7 +20782,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="160"/>
+      <c r="A21" s="162"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -20862,7 +20862,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="156"/>
+      <c r="A23" s="155"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -20901,7 +20901,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
+      <c r="A24" s="158"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -20981,7 +20981,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="156"/>
+      <c r="A26" s="155"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -21020,7 +21020,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
+      <c r="A27" s="158"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -21100,7 +21100,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="156"/>
+      <c r="A29" s="155"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -21139,7 +21139,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="156"/>
+      <c r="A30" s="155"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -21219,7 +21219,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="156"/>
+      <c r="A32" s="155"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -21258,7 +21258,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="156"/>
+      <c r="A33" s="155"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -21338,7 +21338,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="156"/>
+      <c r="A35" s="155"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -21377,7 +21377,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="156"/>
+      <c r="A36" s="155"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -21416,7 +21416,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="157" t="s">
+      <c r="A37" s="156" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -21435,7 +21435,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="157"/>
+      <c r="A38" s="156"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
@@ -21452,7 +21452,7 @@
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="158"/>
+      <c r="A39" s="157"/>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -21470,6 +21470,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A16:A18"/>
@@ -21478,11 +21483,6 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21511,7 +21511,7 @@
       <c r="B1" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="173"/>
+      <c r="C1" s="176"/>
       <c r="D1" s="170" t="s">
         <v>42</v>
       </c>
@@ -21519,19 +21519,19 @@
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="167"/>
       <c r="B2" s="171"/>
-      <c r="C2" s="174"/>
+      <c r="C2" s="177"/>
       <c r="D2" s="171"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="168"/>
       <c r="B3" s="171"/>
-      <c r="C3" s="174"/>
+      <c r="C3" s="177"/>
       <c r="D3" s="171"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="169"/>
       <c r="B4" s="172"/>
-      <c r="C4" s="175"/>
+      <c r="C4" s="178"/>
       <c r="D4" s="172"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21539,7 +21539,7 @@
       <c r="B5" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="176"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="170" t="s">
         <v>43</v>
       </c>
@@ -21547,19 +21547,19 @@
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="167"/>
       <c r="B6" s="171"/>
-      <c r="C6" s="177"/>
+      <c r="C6" s="174"/>
       <c r="D6" s="171"/>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="168"/>
       <c r="B7" s="171"/>
-      <c r="C7" s="177"/>
+      <c r="C7" s="174"/>
       <c r="D7" s="171"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="169"/>
       <c r="B8" s="172"/>
-      <c r="C8" s="178"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="172"/>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21567,7 +21567,7 @@
       <c r="B9" s="170" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="176"/>
+      <c r="C9" s="173"/>
       <c r="D9" s="170" t="s">
         <v>44</v>
       </c>
@@ -21575,19 +21575,19 @@
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="167"/>
       <c r="B10" s="171"/>
-      <c r="C10" s="177"/>
+      <c r="C10" s="174"/>
       <c r="D10" s="171"/>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="168"/>
       <c r="B11" s="171"/>
-      <c r="C11" s="177"/>
+      <c r="C11" s="174"/>
       <c r="D11" s="171"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="169"/>
       <c r="B12" s="172"/>
-      <c r="C12" s="178"/>
+      <c r="C12" s="175"/>
       <c r="D12" s="172"/>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21595,7 +21595,7 @@
       <c r="B13" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="176"/>
+      <c r="C13" s="173"/>
       <c r="D13" s="170" t="s">
         <v>37</v>
       </c>
@@ -21603,19 +21603,19 @@
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="167"/>
       <c r="B14" s="171"/>
-      <c r="C14" s="177"/>
+      <c r="C14" s="174"/>
       <c r="D14" s="171"/>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="168"/>
       <c r="B15" s="171"/>
-      <c r="C15" s="177"/>
+      <c r="C15" s="174"/>
       <c r="D15" s="171"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="169"/>
       <c r="B16" s="172"/>
-      <c r="C16" s="178"/>
+      <c r="C16" s="175"/>
       <c r="D16" s="172"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -21627,6 +21627,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -21635,14 +21643,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21672,7 +21672,7 @@
       <c r="B1" s="179" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="182"/>
+      <c r="C1" s="185"/>
       <c r="D1" s="170" t="s">
         <v>42</v>
       </c>
@@ -21680,19 +21680,19 @@
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="167"/>
       <c r="B2" s="180"/>
-      <c r="C2" s="183"/>
+      <c r="C2" s="186"/>
       <c r="D2" s="171"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="168"/>
       <c r="B3" s="180"/>
-      <c r="C3" s="183"/>
+      <c r="C3" s="186"/>
       <c r="D3" s="171"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="169"/>
       <c r="B4" s="181"/>
-      <c r="C4" s="184"/>
+      <c r="C4" s="187"/>
       <c r="D4" s="172"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21700,7 +21700,7 @@
       <c r="B5" s="179" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="185"/>
+      <c r="C5" s="182"/>
       <c r="D5" s="170" t="s">
         <v>43</v>
       </c>
@@ -21708,19 +21708,19 @@
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="167"/>
       <c r="B6" s="180"/>
-      <c r="C6" s="186"/>
+      <c r="C6" s="183"/>
       <c r="D6" s="171"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="168"/>
       <c r="B7" s="180"/>
-      <c r="C7" s="186"/>
+      <c r="C7" s="183"/>
       <c r="D7" s="171"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="169"/>
       <c r="B8" s="181"/>
-      <c r="C8" s="187"/>
+      <c r="C8" s="184"/>
       <c r="D8" s="172"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21728,7 +21728,7 @@
       <c r="B9" s="179" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="185"/>
+      <c r="C9" s="182"/>
       <c r="D9" s="170" t="s">
         <v>44</v>
       </c>
@@ -21739,21 +21739,21 @@
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="167"/>
       <c r="B10" s="180"/>
-      <c r="C10" s="186"/>
+      <c r="C10" s="183"/>
       <c r="D10" s="171"/>
       <c r="F10" s="171"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="168"/>
       <c r="B11" s="180"/>
-      <c r="C11" s="186"/>
+      <c r="C11" s="183"/>
       <c r="D11" s="171"/>
       <c r="F11" s="171"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="169"/>
       <c r="B12" s="181"/>
-      <c r="C12" s="187"/>
+      <c r="C12" s="184"/>
       <c r="D12" s="172"/>
       <c r="F12" s="172"/>
     </row>
@@ -21762,7 +21762,7 @@
       <c r="B13" s="179" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="185"/>
+      <c r="C13" s="182"/>
       <c r="D13" s="179" t="s">
         <v>37</v>
       </c>
@@ -21773,21 +21773,21 @@
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="167"/>
       <c r="B14" s="180"/>
-      <c r="C14" s="186"/>
+      <c r="C14" s="183"/>
       <c r="D14" s="180"/>
       <c r="G14" s="171"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="168"/>
       <c r="B15" s="180"/>
-      <c r="C15" s="186"/>
+      <c r="C15" s="183"/>
       <c r="D15" s="180"/>
       <c r="G15" s="171"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="169"/>
       <c r="B16" s="181"/>
-      <c r="C16" s="187"/>
+      <c r="C16" s="184"/>
       <c r="D16" s="181"/>
       <c r="G16" s="172"/>
     </row>
@@ -21800,6 +21800,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="G13:G16"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
@@ -21810,14 +21818,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22377,27 +22377,27 @@
       <c r="B1" s="179" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="182"/>
+      <c r="C1" s="185"/>
       <c r="D1" s="179"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="167"/>
       <c r="B2" s="180"/>
-      <c r="C2" s="183"/>
+      <c r="C2" s="186"/>
       <c r="D2" s="180"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="168"/>
       <c r="B3" s="180"/>
-      <c r="C3" s="183"/>
+      <c r="C3" s="186"/>
       <c r="D3" s="180"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="169"/>
       <c r="B4" s="181"/>
-      <c r="C4" s="184"/>
+      <c r="C4" s="187"/>
       <c r="D4" s="181"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -22407,27 +22407,27 @@
       <c r="B5" s="179" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="185"/>
+      <c r="C5" s="182"/>
       <c r="D5" s="170"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="167"/>
       <c r="B6" s="180"/>
-      <c r="C6" s="186"/>
+      <c r="C6" s="183"/>
       <c r="D6" s="171"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="168"/>
       <c r="B7" s="180"/>
-      <c r="C7" s="186"/>
+      <c r="C7" s="183"/>
       <c r="D7" s="171"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="169"/>
       <c r="B8" s="181"/>
-      <c r="C8" s="187"/>
+      <c r="C8" s="184"/>
       <c r="D8" s="172"/>
       <c r="H8"/>
     </row>
@@ -22436,7 +22436,7 @@
       <c r="B9" s="179" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="185"/>
+      <c r="C9" s="182"/>
       <c r="D9" s="170"/>
       <c r="G9"/>
       <c r="H9"/>
@@ -22444,48 +22444,56 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="167"/>
       <c r="B10" s="180"/>
-      <c r="C10" s="186"/>
+      <c r="C10" s="183"/>
       <c r="D10" s="171"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="168"/>
       <c r="B11" s="180"/>
-      <c r="C11" s="186"/>
+      <c r="C11" s="183"/>
       <c r="D11" s="171"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="169"/>
       <c r="B12" s="181"/>
-      <c r="C12" s="187"/>
+      <c r="C12" s="184"/>
       <c r="D12" s="172"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="166"/>
       <c r="B13" s="179"/>
-      <c r="C13" s="185"/>
+      <c r="C13" s="182"/>
       <c r="D13" s="170"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="167"/>
       <c r="B14" s="180"/>
-      <c r="C14" s="186"/>
+      <c r="C14" s="183"/>
       <c r="D14" s="171"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="168"/>
       <c r="B15" s="180"/>
-      <c r="C15" s="186"/>
+      <c r="C15" s="183"/>
       <c r="D15" s="171"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="169"/>
       <c r="B16" s="181"/>
-      <c r="C16" s="187"/>
+      <c r="C16" s="184"/>
       <c r="D16" s="172"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -22494,14 +22502,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22531,7 +22531,7 @@
       <c r="B1" s="179" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="182"/>
+      <c r="C1" s="185"/>
       <c r="D1" s="179" t="s">
         <v>17</v>
       </c>
@@ -22539,20 +22539,20 @@
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="167"/>
       <c r="B2" s="180"/>
-      <c r="C2" s="183"/>
+      <c r="C2" s="186"/>
       <c r="D2" s="180"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="168"/>
       <c r="B3" s="180"/>
-      <c r="C3" s="183"/>
+      <c r="C3" s="186"/>
       <c r="D3" s="180"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="169"/>
       <c r="B4" s="181"/>
-      <c r="C4" s="184"/>
+      <c r="C4" s="187"/>
       <c r="D4" s="181"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -22562,7 +22562,7 @@
       <c r="B5" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="185"/>
+      <c r="C5" s="182"/>
       <c r="D5" s="170" t="s">
         <v>18</v>
       </c>
@@ -22571,19 +22571,19 @@
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="167"/>
       <c r="B6" s="180"/>
-      <c r="C6" s="186"/>
+      <c r="C6" s="183"/>
       <c r="D6" s="171"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="168"/>
       <c r="B7" s="180"/>
-      <c r="C7" s="186"/>
+      <c r="C7" s="183"/>
       <c r="D7" s="171"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="169"/>
       <c r="B8" s="181"/>
-      <c r="C8" s="187"/>
+      <c r="C8" s="184"/>
       <c r="D8" s="172"/>
       <c r="H8"/>
     </row>
@@ -22592,7 +22592,7 @@
       <c r="B9" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="185"/>
+      <c r="C9" s="182"/>
       <c r="D9" s="170" t="s">
         <v>19</v>
       </c>
@@ -22602,19 +22602,19 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="167"/>
       <c r="B10" s="180"/>
-      <c r="C10" s="186"/>
+      <c r="C10" s="183"/>
       <c r="D10" s="171"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="168"/>
       <c r="B11" s="180"/>
-      <c r="C11" s="186"/>
+      <c r="C11" s="183"/>
       <c r="D11" s="171"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="169"/>
       <c r="B12" s="181"/>
-      <c r="C12" s="187"/>
+      <c r="C12" s="184"/>
       <c r="D12" s="172"/>
       <c r="F12"/>
     </row>
@@ -22623,7 +22623,7 @@
       <c r="B13" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="185"/>
+      <c r="C13" s="182"/>
       <c r="D13" s="170" t="s">
         <v>20</v>
       </c>
@@ -22631,23 +22631,31 @@
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="167"/>
       <c r="B14" s="180"/>
-      <c r="C14" s="186"/>
+      <c r="C14" s="183"/>
       <c r="D14" s="171"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="168"/>
       <c r="B15" s="180"/>
-      <c r="C15" s="186"/>
+      <c r="C15" s="183"/>
       <c r="D15" s="171"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="169"/>
       <c r="B16" s="181"/>
-      <c r="C16" s="187"/>
+      <c r="C16" s="184"/>
       <c r="D16" s="172"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -22656,14 +22664,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22693,7 +22693,7 @@
       <c r="B1" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="182"/>
+      <c r="C1" s="185"/>
       <c r="D1" s="170" t="s">
         <v>8</v>
       </c>
@@ -22701,19 +22701,19 @@
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="167"/>
       <c r="B2" s="180"/>
-      <c r="C2" s="183"/>
+      <c r="C2" s="186"/>
       <c r="D2" s="171"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="168"/>
       <c r="B3" s="180"/>
-      <c r="C3" s="183"/>
+      <c r="C3" s="186"/>
       <c r="D3" s="171"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="169"/>
       <c r="B4" s="181"/>
-      <c r="C4" s="184"/>
+      <c r="C4" s="187"/>
       <c r="D4" s="172"/>
       <c r="G4"/>
     </row>
@@ -22722,7 +22722,7 @@
       <c r="B5" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="185"/>
+      <c r="C5" s="182"/>
       <c r="D5" s="170" t="s">
         <v>7</v>
       </c>
@@ -22730,19 +22730,19 @@
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="167"/>
       <c r="B6" s="180"/>
-      <c r="C6" s="186"/>
+      <c r="C6" s="183"/>
       <c r="D6" s="171"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="168"/>
       <c r="B7" s="180"/>
-      <c r="C7" s="186"/>
+      <c r="C7" s="183"/>
       <c r="D7" s="171"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="169"/>
       <c r="B8" s="181"/>
-      <c r="C8" s="187"/>
+      <c r="C8" s="184"/>
       <c r="D8" s="172"/>
       <c r="H8"/>
     </row>
@@ -22751,7 +22751,7 @@
       <c r="B9" s="179" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="185"/>
+      <c r="C9" s="182"/>
       <c r="D9" s="170" t="s">
         <v>9</v>
       </c>
@@ -22759,19 +22759,19 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="167"/>
       <c r="B10" s="180"/>
-      <c r="C10" s="186"/>
+      <c r="C10" s="183"/>
       <c r="D10" s="171"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="168"/>
       <c r="B11" s="180"/>
-      <c r="C11" s="186"/>
+      <c r="C11" s="183"/>
       <c r="D11" s="171"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="169"/>
       <c r="B12" s="181"/>
-      <c r="C12" s="187"/>
+      <c r="C12" s="184"/>
       <c r="D12" s="172"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -22779,29 +22779,37 @@
       <c r="B13" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="185"/>
+      <c r="C13" s="182"/>
       <c r="D13" s="170"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="167"/>
       <c r="B14" s="180"/>
-      <c r="C14" s="186"/>
+      <c r="C14" s="183"/>
       <c r="D14" s="171"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="168"/>
       <c r="B15" s="180"/>
-      <c r="C15" s="186"/>
+      <c r="C15" s="183"/>
       <c r="D15" s="171"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="169"/>
       <c r="B16" s="181"/>
-      <c r="C16" s="187"/>
+      <c r="C16" s="184"/>
       <c r="D16" s="172"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -22810,14 +22818,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22847,7 +22847,7 @@
       <c r="B1" s="179" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="182"/>
+      <c r="C1" s="185"/>
       <c r="D1" s="170" t="s">
         <v>31</v>
       </c>
@@ -22856,20 +22856,20 @@
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="167"/>
       <c r="B2" s="180"/>
-      <c r="C2" s="183"/>
+      <c r="C2" s="186"/>
       <c r="D2" s="171"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="168"/>
       <c r="B3" s="180"/>
-      <c r="C3" s="183"/>
+      <c r="C3" s="186"/>
       <c r="D3" s="171"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="169"/>
       <c r="B4" s="181"/>
-      <c r="C4" s="184"/>
+      <c r="C4" s="187"/>
       <c r="D4" s="172"/>
       <c r="F4"/>
     </row>
@@ -22878,7 +22878,7 @@
       <c r="B5" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="185"/>
+      <c r="C5" s="182"/>
       <c r="D5" s="170" t="s">
         <v>34</v>
       </c>
@@ -22886,20 +22886,20 @@
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="167"/>
       <c r="B6" s="180"/>
-      <c r="C6" s="186"/>
+      <c r="C6" s="183"/>
       <c r="D6" s="171"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="168"/>
       <c r="B7" s="180"/>
-      <c r="C7" s="186"/>
+      <c r="C7" s="183"/>
       <c r="D7" s="171"/>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="169"/>
       <c r="B8" s="181"/>
-      <c r="C8" s="187"/>
+      <c r="C8" s="184"/>
       <c r="D8" s="172"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -22907,7 +22907,7 @@
       <c r="B9" s="179" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="185"/>
+      <c r="C9" s="182"/>
       <c r="D9" s="170" t="s">
         <v>35</v>
       </c>
@@ -22916,25 +22916,25 @@
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="167"/>
       <c r="B10" s="180"/>
-      <c r="C10" s="186"/>
+      <c r="C10" s="183"/>
       <c r="D10" s="171"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="168"/>
       <c r="B11" s="180"/>
-      <c r="C11" s="186"/>
+      <c r="C11" s="183"/>
       <c r="D11" s="171"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="169"/>
       <c r="B12" s="181"/>
-      <c r="C12" s="187"/>
+      <c r="C12" s="184"/>
       <c r="D12" s="172"/>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="166"/>
       <c r="B13" s="179"/>
-      <c r="C13" s="185"/>
+      <c r="C13" s="182"/>
       <c r="D13" s="170" t="s">
         <v>36</v>
       </c>
@@ -22943,23 +22943,31 @@
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="167"/>
       <c r="B14" s="180"/>
-      <c r="C14" s="186"/>
+      <c r="C14" s="183"/>
       <c r="D14" s="171"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="168"/>
       <c r="B15" s="180"/>
-      <c r="C15" s="186"/>
+      <c r="C15" s="183"/>
       <c r="D15" s="171"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="169"/>
       <c r="B16" s="181"/>
-      <c r="C16" s="187"/>
+      <c r="C16" s="184"/>
       <c r="D16" s="172"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -22968,14 +22976,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -23125,13 +23125,13 @@
       <c r="H8" s="49"/>
     </row>
     <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="119" t="s">
+      <c r="A11" s="105" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
     </row>
     <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A12" s="65"/>
@@ -23141,156 +23141,165 @@
       <c r="E12" s="66"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="106" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="120" t="s">
+      <c r="B13" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="105"/>
-      <c r="B14" s="120" t="s">
+      <c r="A14" s="106"/>
+      <c r="B14" s="107" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="105"/>
-      <c r="B15" s="120" t="s">
+      <c r="A15" s="106"/>
+      <c r="B15" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="105"/>
-      <c r="B16" s="120" t="s">
+      <c r="A16" s="106"/>
+      <c r="B16" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="105"/>
-      <c r="B17" s="120" t="s">
+      <c r="A17" s="106"/>
+      <c r="B17" s="107" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="106" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="109"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="111"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="105"/>
-      <c r="B20" s="110"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="112"/>
+      <c r="A20" s="106"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="113"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="114"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="106" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="113" t="s">
+      <c r="B22" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="115"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="117"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="105"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="117"/>
-      <c r="D23" s="117"/>
-      <c r="E23" s="118"/>
+      <c r="A23" s="106"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="105"/>
-      <c r="B24" s="113" t="s">
+      <c r="A24" s="106"/>
+      <c r="B24" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="115"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="117"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="105"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="117"/>
-      <c r="D25" s="117"/>
-      <c r="E25" s="118"/>
+      <c r="A25" s="106"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="120"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="105" t="s">
+      <c r="A27" s="106" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="108" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="106"/>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="105"/>
-      <c r="B28" s="106"/>
-      <c r="C28" s="106"/>
-      <c r="D28" s="106"/>
-      <c r="E28" s="106"/>
+      <c r="A28" s="106"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="105"/>
-      <c r="B29" s="106"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
+      <c r="A29" s="106"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="105" t="s">
+      <c r="A31" s="106" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="108" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="106"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="108"/>
+      <c r="E31" s="108"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="105"/>
-      <c r="B32" s="106"/>
-      <c r="C32" s="106"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
+      <c r="A32" s="106"/>
+      <c r="B32" s="108"/>
+      <c r="C32" s="108"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="108"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="105"/>
-      <c r="B33" s="106"/>
-      <c r="C33" s="106"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="106"/>
+      <c r="A33" s="106"/>
+      <c r="B33" s="108"/>
+      <c r="C33" s="108"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:E29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:E33"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:E20"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:E23"/>
+    <mergeCell ref="B24:E25"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B1:G1"/>
@@ -23301,15 +23310,6 @@
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:E29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:E33"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:E20"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:E23"/>
-    <mergeCell ref="B24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23461,14 +23461,14 @@
       <c r="F10" s="49"/>
     </row>
     <row r="12" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="119" t="s">
+      <c r="A12" s="105" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="119"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A13" s="65"/>
@@ -23479,173 +23479,180 @@
       <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="106" t="s">
         <v>162</v>
       </c>
       <c r="B14" s="70"/>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="105"/>
+      <c r="A15" s="106"/>
       <c r="B15" s="70"/>
-      <c r="C15" s="120" t="s">
+      <c r="C15" s="107" t="s">
         <v>166</v>
       </c>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="105"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="70"/>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
     </row>
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="105"/>
+      <c r="A17" s="106"/>
       <c r="B17" s="70"/>
-      <c r="C17" s="120" t="s">
+      <c r="C17" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
     </row>
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="105"/>
+      <c r="A18" s="106"/>
       <c r="B18" s="70"/>
-      <c r="C18" s="120" t="s">
+      <c r="C18" s="107" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="D18" s="107"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="107"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="106" t="s">
         <v>169</v>
       </c>
       <c r="B20" s="76"/>
-      <c r="C20" s="107" t="s">
+      <c r="C20" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="108"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="109"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="111"/>
     </row>
     <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="105"/>
+      <c r="A21" s="106"/>
       <c r="B21" s="77"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="114"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="105" t="s">
+      <c r="A23" s="106" t="s">
         <v>171</v>
       </c>
       <c r="B23" s="76"/>
-      <c r="C23" s="113" t="s">
+      <c r="C23" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="D23" s="114"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="115"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="117"/>
     </row>
     <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="105"/>
+      <c r="A24" s="106"/>
       <c r="B24" s="77"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="117"/>
-      <c r="E24" s="117"/>
-      <c r="F24" s="118"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="120"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="105"/>
+      <c r="A25" s="106"/>
       <c r="B25" s="76"/>
-      <c r="C25" s="113" t="s">
+      <c r="C25" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="115"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="117"/>
     </row>
     <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="105"/>
+      <c r="A26" s="106"/>
       <c r="B26" s="77"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="117"/>
-      <c r="E26" s="117"/>
-      <c r="F26" s="118"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="120"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="105" t="s">
+      <c r="A28" s="106" t="s">
         <v>174</v>
       </c>
       <c r="B28" s="70"/>
-      <c r="C28" s="106" t="s">
+      <c r="C28" s="108" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="106"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="106"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="108"/>
     </row>
     <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="105"/>
+      <c r="A29" s="106"/>
       <c r="B29" s="70"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="106"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="108"/>
     </row>
     <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="105"/>
+      <c r="A30" s="106"/>
       <c r="B30" s="70"/>
-      <c r="C30" s="106"/>
-      <c r="D30" s="106"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="106"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="108"/>
     </row>
     <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="105" t="s">
+      <c r="A32" s="106" t="s">
         <v>176</v>
       </c>
       <c r="B32" s="70"/>
-      <c r="C32" s="106" t="s">
+      <c r="C32" s="108" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="108"/>
     </row>
     <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="105"/>
+      <c r="A33" s="106"/>
       <c r="B33" s="70"/>
-      <c r="C33" s="106"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="106"/>
+      <c r="C33" s="108"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="108"/>
     </row>
     <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="105"/>
+      <c r="A34" s="106"/>
       <c r="B34" s="70"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="106"/>
+      <c r="C34" s="108"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C28:F30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C32:F34"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="C23:F24"/>
+    <mergeCell ref="C25:F26"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="C3:F3"/>
@@ -23657,13 +23664,6 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C28:F30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C32:F34"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="C23:F24"/>
-    <mergeCell ref="C25:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -24127,12 +24127,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B13:E13"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="A41:E41"/>
@@ -24141,6 +24135,12 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B27:E27"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -24152,7 +24152,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -24258,7 +24258,7 @@
       </c>
       <c r="D5" s="43">
         <f t="shared" ref="D5:D13" si="1">SUM(E5:K5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="44"/>
       <c r="F5" s="44"/>
@@ -24267,7 +24267,9 @@
       </c>
       <c r="H5" s="44"/>
       <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
+      <c r="J5" s="44">
+        <v>1</v>
+      </c>
       <c r="K5" s="44"/>
     </row>
     <row r="6" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24277,7 +24279,7 @@
       </c>
       <c r="D6" s="43">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="44">
         <v>1</v>
@@ -24290,7 +24292,9 @@
       </c>
       <c r="H6" s="44"/>
       <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="J6" s="44">
+        <v>1</v>
+      </c>
       <c r="K6" s="44"/>
     </row>
     <row r="7" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24302,7 +24306,7 @@
       </c>
       <c r="D7" s="43">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="44">
         <v>1</v>
@@ -24312,8 +24316,12 @@
         <v>1</v>
       </c>
       <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
+      <c r="I7" s="44">
+        <v>1</v>
+      </c>
+      <c r="J7" s="44">
+        <v>1</v>
+      </c>
       <c r="K7" s="44"/>
     </row>
     <row r="8" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24380,7 +24388,7 @@
       </c>
       <c r="D11" s="43">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" s="44">
         <v>1</v>
@@ -24393,7 +24401,9 @@
         <v>1</v>
       </c>
       <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
+      <c r="J11" s="44">
+        <v>1</v>
+      </c>
       <c r="K11" s="44"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
@@ -24550,14 +24560,18 @@
       </c>
       <c r="D21" s="43">
         <f>SUM(E21:K21)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="44"/>
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
       <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
+      <c r="I21" s="44">
+        <v>1</v>
+      </c>
+      <c r="J21" s="44">
+        <v>1</v>
+      </c>
       <c r="K21" s="44"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -24579,11 +24593,11 @@
       </c>
       <c r="I22" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Lenovo Ideapad 320, Checkin Timestamp :: Sat 07/16/2022-14:48:17.02;
</commit_message>
<xml_diff>
--- a/My Transformation Journey.xlsx
+++ b/My Transformation Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nc\Awakening-The-Giant-Naresh-Chaurasia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A4F08-765F-474A-8265-CDE941728090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EFF6AE-51C2-4A11-B80C-9E9B88B9782C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="5" xr2:uid="{45287DFE-D99B-4274-A6CA-7DF7915FBBA5}"/>
   </bookViews>
@@ -1562,7 +1562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2069,6 +2069,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2329,7 +2332,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2341,13 +2344,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -2356,7 +2359,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2655,7 +2658,7 @@
             <c:numRef>
               <c:f>'July 10.07.22'!$E$1:$K$1</c:f>
               <c:numCache>
-                <c:formatCode>dd\ mmm</c:formatCode>
+                <c:formatCode>ddd\,\ dd\,\ mmm</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>44752</c:v>
@@ -2703,10 +2706,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2737,7 +2740,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="dd\ mmm" sourceLinked="1"/>
+        <c:numFmt formatCode="ddd\,\ dd\,\ mmm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -24149,10 +24152,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80D2C96-732E-443A-9BBD-AF8FB128AF3B}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -24161,48 +24164,118 @@
     <col min="2" max="2" width="9.140625" style="6"/>
     <col min="3" max="3" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="6"/>
+    <col min="5" max="5" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="6"/>
+    <col min="15" max="15" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="9.140625" style="6"/>
+    <col min="22" max="22" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="9.140625" style="6"/>
+    <col min="26" max="26" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C1" s="46" t="s">
         <v>118</v>
       </c>
       <c r="D1" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="41">
+      <c r="E1" s="188">
         <v>44752</v>
       </c>
-      <c r="F1" s="41">
+      <c r="F1" s="188">
         <f>E1+1</f>
         <v>44753</v>
       </c>
-      <c r="G1" s="41">
+      <c r="G1" s="188">
         <f t="shared" ref="G1:K1" si="0">F1+1</f>
         <v>44754</v>
       </c>
-      <c r="H1" s="41">
+      <c r="H1" s="188">
         <f t="shared" si="0"/>
         <v>44755</v>
       </c>
-      <c r="I1" s="41">
+      <c r="I1" s="188">
         <f t="shared" si="0"/>
         <v>44756</v>
       </c>
-      <c r="J1" s="41">
+      <c r="J1" s="188">
         <f t="shared" si="0"/>
         <v>44757</v>
       </c>
-      <c r="K1" s="41">
+      <c r="K1" s="188">
         <f t="shared" si="0"/>
         <v>44758</v>
       </c>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="188">
+        <f t="shared" ref="L1" si="1">K1+1</f>
+        <v>44759</v>
+      </c>
+      <c r="M1" s="188">
+        <f t="shared" ref="M1" si="2">L1+1</f>
+        <v>44760</v>
+      </c>
+      <c r="N1" s="188">
+        <f t="shared" ref="N1" si="3">M1+1</f>
+        <v>44761</v>
+      </c>
+      <c r="O1" s="188">
+        <f t="shared" ref="O1" si="4">N1+1</f>
+        <v>44762</v>
+      </c>
+      <c r="P1" s="188">
+        <f t="shared" ref="P1" si="5">O1+1</f>
+        <v>44763</v>
+      </c>
+      <c r="Q1" s="188">
+        <f t="shared" ref="Q1" si="6">P1+1</f>
+        <v>44764</v>
+      </c>
+      <c r="R1" s="188">
+        <f t="shared" ref="R1" si="7">Q1+1</f>
+        <v>44765</v>
+      </c>
+      <c r="S1" s="188">
+        <f t="shared" ref="S1" si="8">R1+1</f>
+        <v>44766</v>
+      </c>
+      <c r="T1" s="188">
+        <f t="shared" ref="T1" si="9">S1+1</f>
+        <v>44767</v>
+      </c>
+      <c r="U1" s="188">
+        <f t="shared" ref="U1" si="10">T1+1</f>
+        <v>44768</v>
+      </c>
+      <c r="V1" s="188">
+        <f t="shared" ref="V1" si="11">U1+1</f>
+        <v>44769</v>
+      </c>
+      <c r="W1" s="188">
+        <f t="shared" ref="W1" si="12">V1+1</f>
+        <v>44770</v>
+      </c>
+      <c r="X1" s="188">
+        <f t="shared" ref="X1" si="13">W1+1</f>
+        <v>44771</v>
+      </c>
+      <c r="Y1" s="188">
+        <f t="shared" ref="Y1" si="14">X1+1</f>
+        <v>44772</v>
+      </c>
+      <c r="Z1" s="188">
+        <f t="shared" ref="Z1" si="15">Y1+1</f>
+        <v>44773</v>
+      </c>
+    </row>
+    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B2" s="127">
         <v>1</v>
       </c>
@@ -24220,8 +24293,23 @@
       <c r="I2" s="44"/>
       <c r="J2" s="44"/>
       <c r="K2" s="44"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B3" s="127"/>
       <c r="C3" s="45" t="s">
         <v>127</v>
@@ -24234,8 +24322,23 @@
       <c r="I3" s="44"/>
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
-    </row>
-    <row r="4" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="127"/>
       <c r="C4" s="45" t="s">
         <v>121</v>
@@ -24248,8 +24351,23 @@
       <c r="I4" s="44"/>
       <c r="J4" s="44"/>
       <c r="K4" s="44"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B5" s="128">
         <v>2</v>
       </c>
@@ -24257,7 +24375,7 @@
         <v>116</v>
       </c>
       <c r="D5" s="43">
-        <f t="shared" ref="D5:D13" si="1">SUM(E5:K5)</f>
+        <f t="shared" ref="D5:D13" si="16">SUM(E5:K5)</f>
         <v>2</v>
       </c>
       <c r="E5" s="44"/>
@@ -24271,14 +24389,29 @@
         <v>1</v>
       </c>
       <c r="K5" s="44"/>
-    </row>
-    <row r="6" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="128"/>
       <c r="C6" s="45" t="s">
         <v>124</v>
       </c>
       <c r="D6" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="E6" s="44">
@@ -24296,8 +24429,23 @@
         <v>1</v>
       </c>
       <c r="K6" s="44"/>
-    </row>
-    <row r="7" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="81">
         <v>3</v>
       </c>
@@ -24305,8 +24453,8 @@
         <v>125</v>
       </c>
       <c r="D7" s="43">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="16"/>
+        <v>3</v>
       </c>
       <c r="E7" s="44">
         <v>1</v>
@@ -24319,12 +24467,25 @@
       <c r="I7" s="44">
         <v>1</v>
       </c>
-      <c r="J7" s="44">
-        <v>1</v>
-      </c>
+      <c r="J7" s="44"/>
       <c r="K7" s="44"/>
-    </row>
-    <row r="8" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="129">
         <v>4</v>
       </c>
@@ -24332,7 +24493,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E8" s="44"/>
@@ -24342,14 +24503,29 @@
       <c r="I8" s="44"/>
       <c r="J8" s="44"/>
       <c r="K8" s="44"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" s="129"/>
       <c r="C9" s="86" t="s">
         <v>97</v>
       </c>
       <c r="D9" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E9" s="44"/>
@@ -24359,14 +24535,29 @@
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
       <c r="K9" s="44"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B10" s="129"/>
       <c r="C10" s="45" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="E10" s="44">
@@ -24378,8 +24569,23 @@
       <c r="I10" s="44"/>
       <c r="J10" s="44"/>
       <c r="K10" s="44"/>
-    </row>
-    <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+    </row>
+    <row r="11" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="125">
         <v>5</v>
       </c>
@@ -24387,8 +24593,8 @@
         <v>110</v>
       </c>
       <c r="D11" s="43">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="16"/>
+        <v>5</v>
       </c>
       <c r="E11" s="44">
         <v>1</v>
@@ -24404,15 +24610,32 @@
       <c r="J11" s="44">
         <v>1</v>
       </c>
-      <c r="K11" s="44"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K11" s="44">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12" s="125"/>
       <c r="C12" s="86" t="s">
         <v>131</v>
       </c>
       <c r="D12" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E12" s="44"/>
@@ -24422,8 +24645,23 @@
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
       <c r="K12" s="44"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B13" s="130">
         <v>6</v>
       </c>
@@ -24431,18 +24669,35 @@
         <v>129</v>
       </c>
       <c r="D13" s="43">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>1</v>
       </c>
       <c r="E13" s="44"/>
       <c r="F13" s="44"/>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
       <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
+      <c r="J13" s="44">
+        <v>1</v>
+      </c>
       <c r="K13" s="44"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B14" s="130"/>
       <c r="C14" s="86" t="s">
         <v>117</v>
@@ -24455,8 +24710,23 @@
       <c r="I14" s="44"/>
       <c r="J14" s="44"/>
       <c r="K14" s="44"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B15" s="131">
         <v>7</v>
       </c>
@@ -24471,8 +24741,23 @@
       <c r="I15" s="44"/>
       <c r="J15" s="44"/>
       <c r="K15" s="44"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B16" s="131"/>
       <c r="C16" s="45" t="s">
         <v>1</v>
@@ -24485,8 +24770,23 @@
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
       <c r="K16" s="44"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B17" s="126">
         <v>8</v>
       </c>
@@ -24504,8 +24804,23 @@
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
       <c r="K17" s="44"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B18" s="126"/>
       <c r="C18" s="45" t="s">
         <v>195</v>
@@ -24521,8 +24836,23 @@
       <c r="I18" s="80"/>
       <c r="J18" s="80"/>
       <c r="K18" s="80"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B19" s="82"/>
       <c r="C19" s="86" t="s">
         <v>0</v>
@@ -24535,8 +24865,23 @@
       <c r="I19" s="80"/>
       <c r="J19" s="80"/>
       <c r="K19" s="80"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B20" s="82"/>
       <c r="C20" s="86" t="s">
         <v>54</v>
@@ -24549,8 +24894,23 @@
       <c r="I20" s="80"/>
       <c r="J20" s="80"/>
       <c r="K20" s="80"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="83" t="s">
         <v>196</v>
       </c>
@@ -24560,7 +24920,7 @@
       </c>
       <c r="D21" s="43">
         <f>SUM(E21:K21)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="44"/>
       <c r="F21" s="44"/>
@@ -24569,42 +24929,55 @@
       <c r="I21" s="44">
         <v>1</v>
       </c>
-      <c r="J21" s="44">
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E22" s="7">
+        <f t="shared" ref="E22:K22" si="17">SUM(E4:E21)</f>
+        <v>4</v>
+      </c>
+      <c r="F22" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="K21" s="44"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="7">
-        <f t="shared" ref="E22:K22" si="2">SUM(E4:E21)</f>
+      <c r="I22" s="7">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="F22" s="7">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="G22" s="7">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="H22" s="7">
-        <f t="shared" si="2"/>
+      <c r="K22" s="7">
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="I22" s="7">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J22" s="7">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="K22" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C25" s="46" t="s">
         <v>118</v>
       </c>
@@ -24620,27 +24993,27 @@
         <v>44753</v>
       </c>
       <c r="G25" s="41">
-        <f t="shared" ref="G25" si="3">F25+1</f>
+        <f t="shared" ref="G25" si="18">F25+1</f>
         <v>44754</v>
       </c>
       <c r="H25" s="41">
-        <f t="shared" ref="H25" si="4">G25+1</f>
+        <f t="shared" ref="H25" si="19">G25+1</f>
         <v>44755</v>
       </c>
       <c r="I25" s="41">
-        <f t="shared" ref="I25" si="5">H25+1</f>
+        <f t="shared" ref="I25" si="20">H25+1</f>
         <v>44756</v>
       </c>
       <c r="J25" s="41">
-        <f t="shared" ref="J25" si="6">I25+1</f>
+        <f t="shared" ref="J25" si="21">I25+1</f>
         <v>44757</v>
       </c>
       <c r="K25" s="41">
-        <f t="shared" ref="K25" si="7">J25+1</f>
+        <f t="shared" ref="K25" si="22">J25+1</f>
         <v>44758</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C26" s="45" t="s">
         <v>197</v>
       </c>
@@ -24653,7 +25026,7 @@
       <c r="J26" s="84"/>
       <c r="K26" s="84"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C27" s="45" t="s">
         <v>198</v>
       </c>
@@ -24666,7 +25039,7 @@
       <c r="J27" s="84"/>
       <c r="K27" s="84"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C28" s="45" t="s">
         <v>199</v>
       </c>
@@ -24679,7 +25052,7 @@
       <c r="J28" s="84"/>
       <c r="K28" s="84"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C29" s="45"/>
       <c r="D29" s="43"/>
       <c r="E29" s="84"/>
@@ -24690,7 +25063,7 @@
       <c r="J29" s="84"/>
       <c r="K29" s="84"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C30" s="45"/>
       <c r="D30" s="43"/>
       <c r="E30" s="84"/>
@@ -24701,7 +25074,7 @@
       <c r="J30" s="84"/>
       <c r="K30" s="84"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C31" s="45"/>
       <c r="D31" s="43"/>
       <c r="E31" s="84"/>

</xml_diff>

<commit_message>
Lenovo Ideapad 320, Checkin Timestamp :: Tue 07/19/2022- 9:17:27.07;
</commit_message>
<xml_diff>
--- a/My Transformation Journey.xlsx
+++ b/My Transformation Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nc\Awakening-The-Giant-Naresh-Chaurasia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62025F69-7862-4BDF-AF1A-7DB16F03F354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AA0506-D936-412A-AD05-A882D1EF7A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="5" xr2:uid="{45287DFE-D99B-4274-A6CA-7DF7915FBBA5}"/>
   </bookViews>
@@ -2335,13 +2335,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2371,7 +2371,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -2383,7 +2383,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -24179,7 +24179,7 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA32" sqref="AA32"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -24407,7 +24407,7 @@
       </c>
       <c r="D5" s="43">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="44"/>
@@ -24423,7 +24423,9 @@
         <v>1</v>
       </c>
       <c r="L5" s="22"/>
-      <c r="M5" s="90"/>
+      <c r="M5" s="90">
+        <v>1</v>
+      </c>
       <c r="N5" s="90"/>
       <c r="O5" s="90"/>
       <c r="P5" s="90"/>
@@ -24487,7 +24489,7 @@
       </c>
       <c r="D7" s="43">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="22">
         <v>1</v>
@@ -24507,7 +24509,9 @@
       <c r="L7" s="22">
         <v>1</v>
       </c>
-      <c r="M7" s="90"/>
+      <c r="M7" s="90">
+        <v>1</v>
+      </c>
       <c r="N7" s="90"/>
       <c r="O7" s="90"/>
       <c r="P7" s="90"/>
@@ -24843,7 +24847,7 @@
       </c>
       <c r="D17" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="44"/>
@@ -24853,7 +24857,9 @@
       <c r="J17" s="44"/>
       <c r="K17" s="44"/>
       <c r="L17" s="22"/>
-      <c r="M17" s="90"/>
+      <c r="M17" s="90">
+        <v>1</v>
+      </c>
       <c r="N17" s="90"/>
       <c r="O17" s="90"/>
       <c r="P17" s="90"/>
@@ -24974,7 +24980,7 @@
       </c>
       <c r="D21" s="43">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="44"/>
@@ -24986,7 +24992,9 @@
       <c r="J21" s="44"/>
       <c r="K21" s="44"/>
       <c r="L21" s="22"/>
-      <c r="M21" s="90"/>
+      <c r="M21" s="90">
+        <v>1</v>
+      </c>
       <c r="N21" s="90"/>
       <c r="O21" s="90"/>
       <c r="P21" s="90"/>

</xml_diff>

<commit_message>
Lenovo Ideapad 320, Checkin Timestamp :: Mon 07/25/2022-16:55:47.23;
</commit_message>
<xml_diff>
--- a/My Transformation Journey.xlsx
+++ b/My Transformation Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nc\Awakening-The-Giant-Naresh-Chaurasia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A222AE47-38A5-43CA-B04E-ADEA190012C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FF921F-09F1-41F6-A8ED-E4B73FB1DFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="5" xr2:uid="{45287DFE-D99B-4274-A6CA-7DF7915FBBA5}"/>
   </bookViews>
@@ -2341,10 +2341,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2695,10 +2695,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'July 10.07.22'!$E$1:$K$1</c:f>
+              <c:f>'July 10.07.22'!$E$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>ddd\,\ dd\,\ mmm</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>44752</c:v>
                 </c:pt>
@@ -2720,15 +2720,60 @@
                 <c:pt idx="6">
                   <c:v>44758</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>44759</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44760</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44761</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44762</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44763</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44765</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44766</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44767</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44769</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44770</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44771</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44772</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44773</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'July 10.07.22'!$E$22:$K$22</c:f>
+              <c:f>'July 10.07.22'!$E$22:$Z$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -2749,6 +2794,48 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7583,8 +7670,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -7621,14 +7708,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>9523</xdr:rowOff>
     </xdr:to>
@@ -23354,7 +23441,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -23487,7 +23574,7 @@
       </c>
       <c r="D2" s="43">
         <f>SUM(E2:Z2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="44"/>
@@ -23505,7 +23592,7 @@
       <c r="R2" s="89"/>
       <c r="S2" s="89"/>
       <c r="T2" s="89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U2" s="89"/>
       <c r="V2" s="89"/>
@@ -23524,7 +23611,7 @@
       </c>
       <c r="D3" s="43">
         <f t="shared" ref="D3:D21" si="16">SUM(E3:Z3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="44"/>
@@ -23541,7 +23628,9 @@
       <c r="Q3" s="89"/>
       <c r="R3" s="89"/>
       <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
+      <c r="T3" s="89">
+        <v>1</v>
+      </c>
       <c r="U3" s="89"/>
       <c r="V3" s="89"/>
       <c r="W3" s="89"/>
@@ -24212,7 +24301,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E22" s="7">
-        <f t="shared" ref="E22:K22" si="17">SUM(E4:E21)</f>
+        <f t="shared" ref="E22:Z22" si="17">SUM(E4:E21)</f>
         <v>4</v>
       </c>
       <c r="F22" s="7">
@@ -24238,6 +24327,62 @@
       <c r="K22" s="7">
         <f t="shared" si="17"/>
         <v>3</v>
+      </c>
+      <c r="M22" s="7">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="N22" s="7">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="7">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="R22" s="7">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="S22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="7">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="U22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lenovo Ideapad 320, Checkin Timestamp :: Thu 07/28/2022-14:19:28.92;
</commit_message>
<xml_diff>
--- a/My Transformation Journey.xlsx
+++ b/My Transformation Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nc\Awakening-The-Giant-Naresh-Chaurasia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FF921F-09F1-41F6-A8ED-E4B73FB1DFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73D541C-74D7-4D92-88C7-48504BDFDB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2205" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="5" xr2:uid="{45287DFE-D99B-4274-A6CA-7DF7915FBBA5}"/>
   </bookViews>
@@ -1787,12 +1787,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1804,6 +1798,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1832,14 +1832,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1879,6 +1873,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1982,6 +1982,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1991,15 +1994,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2007,6 +2001,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2037,6 +2037,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2044,15 +2053,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2064,6 +2064,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2071,15 +2080,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2341,10 +2341,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2356,7 +2356,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2368,7 +2368,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2377,7 +2377,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -2389,16 +2389,16 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2698,71 +2698,20 @@
               <c:f>'July 10.07.22'!$E$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>ddd\,\ dd\,\ mmm</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>44752</c:v>
+                  <c:v>44769</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44753</c:v>
+                  <c:v>44770</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44754</c:v>
+                  <c:v>44771</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44755</c:v>
+                  <c:v>44772</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44756</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44757</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44758</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44759</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44760</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44761</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44762</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44763</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44764</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44765</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44766</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44767</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44768</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44769</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44770</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44771</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44772</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>44773</c:v>
                 </c:pt>
               </c:numCache>
@@ -2773,68 +2722,20 @@
               <c:f>'July 10.07.22'!$E$22:$Z$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -10901,10 +10802,10 @@
       <c r="A1" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="92" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="95"/>
+      <c r="C1" s="93"/>
       <c r="D1" s="88">
         <v>5</v>
       </c>
@@ -10947,10 +10848,10 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="87"/>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="94" t="s">
         <v>196</v>
       </c>
-      <c r="C2" s="97"/>
+      <c r="C2" s="95"/>
       <c r="D2" s="88"/>
       <c r="E2" s="88"/>
       <c r="F2" s="88"/>
@@ -10966,8 +10867,8 @@
       <c r="A3" s="86">
         <v>44753</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="93"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="97"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="84"/>
@@ -10984,8 +10885,8 @@
         <f>A3+1</f>
         <v>44754</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="93"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="97"/>
       <c r="D4" s="84"/>
       <c r="E4" s="84"/>
       <c r="F4" s="84"/>
@@ -11002,8 +10903,8 @@
         <f t="shared" ref="A5:A23" si="1">A4+1</f>
         <v>44755</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="93"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="97"/>
       <c r="D5" s="84"/>
       <c r="E5" s="84"/>
       <c r="F5" s="84"/>
@@ -11020,8 +10921,8 @@
         <f t="shared" si="1"/>
         <v>44756</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="97"/>
       <c r="D6" s="84"/>
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
@@ -11038,8 +10939,8 @@
         <f t="shared" si="1"/>
         <v>44757</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="93"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="97"/>
       <c r="D7" s="84"/>
       <c r="E7" s="84"/>
       <c r="F7" s="84"/>
@@ -11056,8 +10957,8 @@
         <f t="shared" si="1"/>
         <v>44758</v>
       </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="93"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="97"/>
       <c r="D8" s="84"/>
       <c r="E8" s="84"/>
       <c r="F8" s="84"/>
@@ -11074,8 +10975,8 @@
         <f t="shared" si="1"/>
         <v>44759</v>
       </c>
-      <c r="B9" s="92"/>
-      <c r="C9" s="93"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="84"/>
       <c r="E9" s="84"/>
       <c r="F9" s="84"/>
@@ -11092,8 +10993,8 @@
         <f t="shared" si="1"/>
         <v>44760</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="93"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="84"/>
       <c r="E10" s="84"/>
       <c r="F10" s="84"/>
@@ -11110,8 +11011,8 @@
         <f t="shared" si="1"/>
         <v>44761</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="93"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="84"/>
       <c r="E11" s="84"/>
       <c r="F11" s="84"/>
@@ -11128,8 +11029,8 @@
         <f t="shared" si="1"/>
         <v>44762</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="93"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
       <c r="F12" s="84"/>
@@ -11146,8 +11047,8 @@
         <f t="shared" si="1"/>
         <v>44763</v>
       </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="93"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="84"/>
       <c r="E13" s="84"/>
       <c r="F13" s="84"/>
@@ -11164,8 +11065,8 @@
         <f t="shared" si="1"/>
         <v>44764</v>
       </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="93"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="97"/>
       <c r="D14" s="84"/>
       <c r="E14" s="84"/>
       <c r="F14" s="84"/>
@@ -11182,8 +11083,8 @@
         <f t="shared" si="1"/>
         <v>44765</v>
       </c>
-      <c r="B15" s="92"/>
-      <c r="C15" s="93"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="97"/>
       <c r="D15" s="84"/>
       <c r="E15" s="84"/>
       <c r="F15" s="84"/>
@@ -11200,8 +11101,8 @@
         <f t="shared" si="1"/>
         <v>44766</v>
       </c>
-      <c r="B16" s="92"/>
-      <c r="C16" s="93"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
       <c r="D16" s="84"/>
       <c r="E16" s="84"/>
       <c r="F16" s="84"/>
@@ -11218,8 +11119,8 @@
         <f t="shared" si="1"/>
         <v>44767</v>
       </c>
-      <c r="B17" s="92"/>
-      <c r="C17" s="93"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
       <c r="F17" s="84"/>
@@ -11236,8 +11137,8 @@
         <f t="shared" si="1"/>
         <v>44768</v>
       </c>
-      <c r="B18" s="92"/>
-      <c r="C18" s="93"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="84"/>
       <c r="E18" s="84"/>
       <c r="F18" s="84"/>
@@ -11254,8 +11155,8 @@
         <f t="shared" si="1"/>
         <v>44769</v>
       </c>
-      <c r="B19" s="92"/>
-      <c r="C19" s="93"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="97"/>
       <c r="D19" s="84"/>
       <c r="E19" s="84"/>
       <c r="F19" s="84"/>
@@ -11272,8 +11173,8 @@
         <f>A19+1</f>
         <v>44770</v>
       </c>
-      <c r="B20" s="92"/>
-      <c r="C20" s="93"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
       <c r="D20" s="84"/>
       <c r="E20" s="84"/>
       <c r="F20" s="84"/>
@@ -11290,8 +11191,8 @@
         <f t="shared" si="1"/>
         <v>44771</v>
       </c>
-      <c r="B21" s="92"/>
-      <c r="C21" s="93"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="97"/>
       <c r="D21" s="84"/>
       <c r="E21" s="84"/>
       <c r="F21" s="84"/>
@@ -11308,8 +11209,8 @@
         <f t="shared" si="1"/>
         <v>44772</v>
       </c>
-      <c r="B22" s="92"/>
-      <c r="C22" s="93"/>
+      <c r="B22" s="96"/>
+      <c r="C22" s="97"/>
       <c r="D22" s="84"/>
       <c r="E22" s="84"/>
       <c r="F22" s="84"/>
@@ -11326,8 +11227,8 @@
         <f t="shared" si="1"/>
         <v>44773</v>
       </c>
-      <c r="B23" s="92"/>
-      <c r="C23" s="93"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="97"/>
       <c r="D23" s="84"/>
       <c r="E23" s="84"/>
       <c r="F23" s="84"/>
@@ -11341,6 +11242,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B21:C21"/>
@@ -11357,13 +11265,6 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12213,7 +12114,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -12232,7 +12133,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="158"/>
+      <c r="A2" s="159"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -12249,7 +12150,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="159"/>
+      <c r="A3" s="160"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -12307,7 +12208,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="160"/>
+      <c r="A5" s="157"/>
       <c r="B5" s="18" t="s">
         <v>29</v>
       </c>
@@ -12387,7 +12288,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="160"/>
+      <c r="A7" s="157"/>
       <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
@@ -12467,7 +12368,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="157"/>
+      <c r="A9" s="158"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -12547,7 +12448,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="157"/>
+      <c r="A11" s="158"/>
       <c r="B11" s="18" t="s">
         <v>29</v>
       </c>
@@ -12627,7 +12528,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="157"/>
+      <c r="A13" s="158"/>
       <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
@@ -12707,7 +12608,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="157"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -12787,7 +12688,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="157"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="18" t="s">
         <v>29</v>
       </c>
@@ -12867,7 +12768,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="160"/>
+      <c r="A19" s="157"/>
       <c r="B19" s="18" t="s">
         <v>29</v>
       </c>
@@ -12947,7 +12848,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="157"/>
+      <c r="A21" s="158"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -13027,7 +12928,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="157"/>
+      <c r="A23" s="158"/>
       <c r="B23" s="18" t="s">
         <v>29</v>
       </c>
@@ -13107,7 +13008,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="160"/>
+      <c r="A25" s="157"/>
       <c r="B25" s="18" t="s">
         <v>29</v>
       </c>
@@ -13187,7 +13088,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="160"/>
+      <c r="A27" s="157"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -13267,7 +13168,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="160"/>
+      <c r="A29" s="157"/>
       <c r="B29" s="18" t="s">
         <v>29</v>
       </c>
@@ -13347,7 +13248,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="160"/>
+      <c r="A31" s="157"/>
       <c r="B31" s="18" t="s">
         <v>29</v>
       </c>
@@ -13387,6 +13288,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -13396,12 +13303,6 @@
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -13425,7 +13326,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -13444,7 +13345,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="158"/>
+      <c r="A2" s="159"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -13461,7 +13362,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="159"/>
+      <c r="A3" s="160"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -13519,7 +13420,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="157"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -13558,7 +13459,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="160"/>
+      <c r="A6" s="157"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -13638,7 +13539,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="157"/>
+      <c r="A8" s="158"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -13677,7 +13578,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
+      <c r="A9" s="157"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -13716,7 +13617,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="164" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -13757,7 +13658,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="162"/>
+      <c r="A11" s="165"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -13796,7 +13697,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="162"/>
+      <c r="A12" s="165"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -13876,7 +13777,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="157"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -13915,7 +13816,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="160"/>
+      <c r="A15" s="157"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -13995,7 +13896,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="157"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -14034,7 +13935,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="160"/>
+      <c r="A18" s="157"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -14073,7 +13974,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="161" t="s">
+      <c r="A19" s="164" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -14114,7 +14015,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="162"/>
+      <c r="A20" s="165"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -14153,7 +14054,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="162"/>
+      <c r="A21" s="165"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -14233,7 +14134,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="157"/>
+      <c r="A23" s="158"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -14272,7 +14173,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="160"/>
+      <c r="A24" s="157"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -14352,7 +14253,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="157"/>
+      <c r="A26" s="158"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -14391,7 +14292,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="160"/>
+      <c r="A27" s="157"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -14430,7 +14331,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="163"/>
+      <c r="A28" s="161"/>
       <c r="B28" s="16" t="s">
         <v>29</v>
       </c>
@@ -14469,7 +14370,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="164"/>
+      <c r="A29" s="162"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -14508,7 +14409,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="164"/>
+      <c r="A30" s="162"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -14547,7 +14448,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="163"/>
+      <c r="A31" s="161"/>
       <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
@@ -14586,7 +14487,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="164"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -14625,7 +14526,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="165"/>
+      <c r="A33" s="163"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -14664,7 +14565,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="163"/>
+      <c r="A34" s="161"/>
       <c r="B34" s="16" t="s">
         <v>29</v>
       </c>
@@ -14703,7 +14604,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="164"/>
+      <c r="A35" s="162"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -14742,7 +14643,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="165"/>
+      <c r="A36" s="163"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -14781,7 +14682,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="163"/>
+      <c r="A37" s="161"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
@@ -14820,7 +14721,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="164"/>
+      <c r="A38" s="162"/>
       <c r="B38" s="17" t="s">
         <v>29</v>
       </c>
@@ -14859,7 +14760,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="165"/>
+      <c r="A39" s="163"/>
       <c r="B39" s="18" t="s">
         <v>29</v>
       </c>
@@ -14899,6 +14800,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -14906,12 +14813,6 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -15029,7 +14930,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="157"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -15068,7 +14969,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="160"/>
+      <c r="A6" s="157"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -15148,7 +15049,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="157"/>
+      <c r="A8" s="158"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -15187,7 +15088,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
+      <c r="A9" s="157"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -15267,7 +15168,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="157"/>
+      <c r="A11" s="158"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -15306,7 +15207,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="157"/>
+      <c r="A12" s="158"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -15386,7 +15287,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="157"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -15425,7 +15326,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="157"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -15505,7 +15406,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="157"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -15544,7 +15445,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="157"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -15622,7 +15523,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="157"/>
+      <c r="A20" s="158"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -15661,7 +15562,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="157"/>
+      <c r="A21" s="158"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -15741,7 +15642,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="157"/>
+      <c r="A23" s="158"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -15780,7 +15681,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="160"/>
+      <c r="A24" s="157"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -15860,7 +15761,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="157"/>
+      <c r="A26" s="158"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -15899,7 +15800,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="160"/>
+      <c r="A27" s="157"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -15979,7 +15880,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="157"/>
+      <c r="A29" s="158"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -16018,7 +15919,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="160"/>
+      <c r="A30" s="157"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -16098,7 +15999,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="157"/>
+      <c r="A32" s="158"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -16137,7 +16038,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="160"/>
+      <c r="A33" s="157"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -16217,7 +16118,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="157"/>
+      <c r="A35" s="158"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -16256,7 +16157,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="160"/>
+      <c r="A36" s="157"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -16385,7 +16286,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -16404,7 +16305,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="158"/>
+      <c r="A2" s="159"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -16421,7 +16322,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="159"/>
+      <c r="A3" s="160"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -16479,7 +16380,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="157"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -16518,7 +16419,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="160"/>
+      <c r="A6" s="157"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -16598,7 +16499,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="157"/>
+      <c r="A8" s="158"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -16637,7 +16538,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
+      <c r="A9" s="157"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -16717,7 +16618,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="157"/>
+      <c r="A11" s="158"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -16756,7 +16657,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="157"/>
+      <c r="A12" s="158"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -16836,7 +16737,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="157"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -16875,7 +16776,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="157"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -16955,7 +16856,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="157"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -16994,7 +16895,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="157"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -17033,7 +16934,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="163"/>
+      <c r="A19" s="161"/>
       <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
@@ -17072,7 +16973,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="164"/>
+      <c r="A20" s="162"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -17111,7 +17012,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="164"/>
+      <c r="A21" s="162"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -17191,7 +17092,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="157"/>
+      <c r="A23" s="158"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -17230,7 +17131,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="160"/>
+      <c r="A24" s="157"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -17310,7 +17211,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="157"/>
+      <c r="A26" s="158"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -17349,7 +17250,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="160"/>
+      <c r="A27" s="157"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -17429,7 +17330,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="157"/>
+      <c r="A29" s="158"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -17468,7 +17369,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="157"/>
+      <c r="A30" s="158"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -17548,7 +17449,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="157"/>
+      <c r="A32" s="158"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -17587,7 +17488,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="157"/>
+      <c r="A33" s="158"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -17667,7 +17568,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="157"/>
+      <c r="A35" s="158"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -17706,7 +17607,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="160"/>
+      <c r="A36" s="157"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -17745,7 +17646,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="158" t="s">
+      <c r="A37" s="159" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -17764,7 +17665,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="158"/>
+      <c r="A38" s="159"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
@@ -17781,7 +17682,7 @@
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="159"/>
+      <c r="A39" s="160"/>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -17799,6 +17700,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -17806,12 +17713,6 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -17835,7 +17736,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -17854,7 +17755,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="158"/>
+      <c r="A2" s="159"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -17871,7 +17772,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="159"/>
+      <c r="A3" s="160"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -17929,7 +17830,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="157"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -17968,7 +17869,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="160"/>
+      <c r="A6" s="157"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -18048,7 +17949,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="157"/>
+      <c r="A8" s="158"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -18087,7 +17988,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
+      <c r="A9" s="157"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -18167,7 +18068,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="157"/>
+      <c r="A11" s="158"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -18206,7 +18107,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="157"/>
+      <c r="A12" s="158"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -18286,7 +18187,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="157"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -18325,7 +18226,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="157"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -18405,7 +18306,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="157"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -18444,7 +18345,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="157"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -18524,7 +18425,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="157"/>
+      <c r="A20" s="158"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -18563,7 +18464,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="157"/>
+      <c r="A21" s="158"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -18643,7 +18544,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="157"/>
+      <c r="A23" s="158"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -18682,7 +18583,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="157"/>
+      <c r="A24" s="158"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -18762,7 +18663,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="157"/>
+      <c r="A26" s="158"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -18801,7 +18702,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="160"/>
+      <c r="A27" s="157"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -18840,7 +18741,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="163"/>
+      <c r="A28" s="161"/>
       <c r="B28" s="16" t="s">
         <v>29</v>
       </c>
@@ -18879,7 +18780,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="164"/>
+      <c r="A29" s="162"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -18918,7 +18819,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="164"/>
+      <c r="A30" s="162"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -18957,7 +18858,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="163"/>
+      <c r="A31" s="161"/>
       <c r="B31" s="16" t="s">
         <v>29</v>
       </c>
@@ -18996,7 +18897,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="164"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -19035,7 +18936,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="164"/>
+      <c r="A33" s="162"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -19074,7 +18975,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="163"/>
+      <c r="A34" s="161"/>
       <c r="B34" s="16" t="s">
         <v>29</v>
       </c>
@@ -19113,7 +19014,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="164"/>
+      <c r="A35" s="162"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -19152,7 +19053,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="165"/>
+      <c r="A36" s="163"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -19191,7 +19092,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="163"/>
+      <c r="A37" s="161"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
@@ -19230,7 +19131,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="164"/>
+      <c r="A38" s="162"/>
       <c r="B38" s="17" t="s">
         <v>29</v>
       </c>
@@ -19269,7 +19170,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="165"/>
+      <c r="A39" s="163"/>
       <c r="B39" s="18" t="s">
         <v>29</v>
       </c>
@@ -19309,6 +19210,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
@@ -19316,12 +19223,6 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -19345,7 +19246,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -19364,7 +19265,7 @@
       <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="158"/>
+      <c r="A2" s="159"/>
       <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
@@ -19381,7 +19282,7 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="159"/>
+      <c r="A3" s="160"/>
       <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
@@ -19439,7 +19340,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="157"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
@@ -19478,7 +19379,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="160"/>
+      <c r="A6" s="157"/>
       <c r="B6" s="18" t="s">
         <v>29</v>
       </c>
@@ -19558,7 +19459,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="157"/>
+      <c r="A8" s="158"/>
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
@@ -19597,7 +19498,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
+      <c r="A9" s="157"/>
       <c r="B9" s="18" t="s">
         <v>29</v>
       </c>
@@ -19677,7 +19578,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="157"/>
+      <c r="A11" s="158"/>
       <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
@@ -19716,7 +19617,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="157"/>
+      <c r="A12" s="158"/>
       <c r="B12" s="18" t="s">
         <v>29</v>
       </c>
@@ -19796,7 +19697,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="157"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
@@ -19835,7 +19736,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="157"/>
+      <c r="A15" s="158"/>
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -19915,7 +19816,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="157"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="17" t="s">
         <v>29</v>
       </c>
@@ -19954,7 +19855,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="157"/>
+      <c r="A18" s="158"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -19993,7 +19894,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="163"/>
+      <c r="A19" s="161"/>
       <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
@@ -20032,7 +19933,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="164"/>
+      <c r="A20" s="162"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
@@ -20071,7 +19972,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="164"/>
+      <c r="A21" s="162"/>
       <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
@@ -20151,7 +20052,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="157"/>
+      <c r="A23" s="158"/>
       <c r="B23" s="17" t="s">
         <v>29</v>
       </c>
@@ -20190,7 +20091,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="160"/>
+      <c r="A24" s="157"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
@@ -20270,7 +20171,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="157"/>
+      <c r="A26" s="158"/>
       <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
@@ -20309,7 +20210,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="160"/>
+      <c r="A27" s="157"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -20389,7 +20290,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="157"/>
+      <c r="A29" s="158"/>
       <c r="B29" s="17" t="s">
         <v>29</v>
       </c>
@@ -20428,7 +20329,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="157"/>
+      <c r="A30" s="158"/>
       <c r="B30" s="18" t="s">
         <v>29</v>
       </c>
@@ -20508,7 +20409,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="157"/>
+      <c r="A32" s="158"/>
       <c r="B32" s="17" t="s">
         <v>29</v>
       </c>
@@ -20547,7 +20448,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="157"/>
+      <c r="A33" s="158"/>
       <c r="B33" s="18" t="s">
         <v>29</v>
       </c>
@@ -20627,7 +20528,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="157"/>
+      <c r="A35" s="158"/>
       <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
@@ -20666,7 +20567,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="157"/>
+      <c r="A36" s="158"/>
       <c r="B36" s="18" t="s">
         <v>29</v>
       </c>
@@ -20705,7 +20606,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="158" t="s">
+      <c r="A37" s="159" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -20724,7 +20625,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="158"/>
+      <c r="A38" s="159"/>
       <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
@@ -20741,7 +20642,7 @@
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="159"/>
+      <c r="A39" s="160"/>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -20759,11 +20660,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A16:A18"/>
@@ -20772,6 +20668,11 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -20800,7 +20701,7 @@
       <c r="B1" s="172" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="178"/>
+      <c r="C1" s="175"/>
       <c r="D1" s="172" t="s">
         <v>42</v>
       </c>
@@ -20808,19 +20709,19 @@
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="169"/>
       <c r="B2" s="173"/>
-      <c r="C2" s="179"/>
+      <c r="C2" s="176"/>
       <c r="D2" s="173"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="170"/>
       <c r="B3" s="173"/>
-      <c r="C3" s="179"/>
+      <c r="C3" s="176"/>
       <c r="D3" s="173"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="171"/>
       <c r="B4" s="174"/>
-      <c r="C4" s="180"/>
+      <c r="C4" s="177"/>
       <c r="D4" s="174"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -20828,7 +20729,7 @@
       <c r="B5" s="172" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="175"/>
+      <c r="C5" s="178"/>
       <c r="D5" s="172" t="s">
         <v>43</v>
       </c>
@@ -20836,19 +20737,19 @@
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="169"/>
       <c r="B6" s="173"/>
-      <c r="C6" s="176"/>
+      <c r="C6" s="179"/>
       <c r="D6" s="173"/>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="170"/>
       <c r="B7" s="173"/>
-      <c r="C7" s="176"/>
+      <c r="C7" s="179"/>
       <c r="D7" s="173"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="171"/>
       <c r="B8" s="174"/>
-      <c r="C8" s="177"/>
+      <c r="C8" s="180"/>
       <c r="D8" s="174"/>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -20856,7 +20757,7 @@
       <c r="B9" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="175"/>
+      <c r="C9" s="178"/>
       <c r="D9" s="172" t="s">
         <v>44</v>
       </c>
@@ -20864,19 +20765,19 @@
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="169"/>
       <c r="B10" s="173"/>
-      <c r="C10" s="176"/>
+      <c r="C10" s="179"/>
       <c r="D10" s="173"/>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="170"/>
       <c r="B11" s="173"/>
-      <c r="C11" s="176"/>
+      <c r="C11" s="179"/>
       <c r="D11" s="173"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="171"/>
       <c r="B12" s="174"/>
-      <c r="C12" s="177"/>
+      <c r="C12" s="180"/>
       <c r="D12" s="174"/>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -20884,7 +20785,7 @@
       <c r="B13" s="172" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="175"/>
+      <c r="C13" s="178"/>
       <c r="D13" s="172" t="s">
         <v>37</v>
       </c>
@@ -20892,19 +20793,19 @@
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="169"/>
       <c r="B14" s="173"/>
-      <c r="C14" s="176"/>
+      <c r="C14" s="179"/>
       <c r="D14" s="173"/>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="170"/>
       <c r="B15" s="173"/>
-      <c r="C15" s="176"/>
+      <c r="C15" s="179"/>
       <c r="D15" s="173"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="171"/>
       <c r="B16" s="174"/>
-      <c r="C16" s="177"/>
+      <c r="C16" s="180"/>
       <c r="D16" s="174"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -20916,6 +20817,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -20924,14 +20833,6 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -20961,7 +20862,7 @@
       <c r="B1" s="181" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="187"/>
+      <c r="C1" s="184"/>
       <c r="D1" s="172" t="s">
         <v>42</v>
       </c>
@@ -20969,19 +20870,19 @@
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="169"/>
       <c r="B2" s="182"/>
-      <c r="C2" s="188"/>
+      <c r="C2" s="185"/>
       <c r="D2" s="173"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="170"/>
       <c r="B3" s="182"/>
-      <c r="C3" s="188"/>
+      <c r="C3" s="185"/>
       <c r="D3" s="173"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="171"/>
       <c r="B4" s="183"/>
-      <c r="C4" s="189"/>
+      <c r="C4" s="186"/>
       <c r="D4" s="174"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -20989,7 +20890,7 @@
       <c r="B5" s="181" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="184"/>
+      <c r="C5" s="187"/>
       <c r="D5" s="172" t="s">
         <v>43</v>
       </c>
@@ -20997,19 +20898,19 @@
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="169"/>
       <c r="B6" s="182"/>
-      <c r="C6" s="185"/>
+      <c r="C6" s="188"/>
       <c r="D6" s="173"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="170"/>
       <c r="B7" s="182"/>
-      <c r="C7" s="185"/>
+      <c r="C7" s="188"/>
       <c r="D7" s="173"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="171"/>
       <c r="B8" s="183"/>
-      <c r="C8" s="186"/>
+      <c r="C8" s="189"/>
       <c r="D8" s="174"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21017,7 +20918,7 @@
       <c r="B9" s="181" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="184"/>
+      <c r="C9" s="187"/>
       <c r="D9" s="172" t="s">
         <v>44</v>
       </c>
@@ -21028,21 +20929,21 @@
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="169"/>
       <c r="B10" s="182"/>
-      <c r="C10" s="185"/>
+      <c r="C10" s="188"/>
       <c r="D10" s="173"/>
       <c r="F10" s="173"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="170"/>
       <c r="B11" s="182"/>
-      <c r="C11" s="185"/>
+      <c r="C11" s="188"/>
       <c r="D11" s="173"/>
       <c r="F11" s="173"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="171"/>
       <c r="B12" s="183"/>
-      <c r="C12" s="186"/>
+      <c r="C12" s="189"/>
       <c r="D12" s="174"/>
       <c r="F12" s="174"/>
     </row>
@@ -21051,7 +20952,7 @@
       <c r="B13" s="181" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="184"/>
+      <c r="C13" s="187"/>
       <c r="D13" s="181" t="s">
         <v>37</v>
       </c>
@@ -21062,21 +20963,21 @@
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="169"/>
       <c r="B14" s="182"/>
-      <c r="C14" s="185"/>
+      <c r="C14" s="188"/>
       <c r="D14" s="182"/>
       <c r="G14" s="173"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="170"/>
       <c r="B15" s="182"/>
-      <c r="C15" s="185"/>
+      <c r="C15" s="188"/>
       <c r="D15" s="182"/>
       <c r="G15" s="173"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="171"/>
       <c r="B16" s="183"/>
-      <c r="C16" s="186"/>
+      <c r="C16" s="189"/>
       <c r="D16" s="183"/>
       <c r="G16" s="174"/>
     </row>
@@ -21089,14 +20990,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
     <mergeCell ref="G13:G16"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
@@ -21107,6 +21000,14 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21666,27 +21567,27 @@
       <c r="B1" s="181" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="187"/>
+      <c r="C1" s="184"/>
       <c r="D1" s="181"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="169"/>
       <c r="B2" s="182"/>
-      <c r="C2" s="188"/>
+      <c r="C2" s="185"/>
       <c r="D2" s="182"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="170"/>
       <c r="B3" s="182"/>
-      <c r="C3" s="188"/>
+      <c r="C3" s="185"/>
       <c r="D3" s="182"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="171"/>
       <c r="B4" s="183"/>
-      <c r="C4" s="189"/>
+      <c r="C4" s="186"/>
       <c r="D4" s="183"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -21696,27 +21597,27 @@
       <c r="B5" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="184"/>
+      <c r="C5" s="187"/>
       <c r="D5" s="172"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="169"/>
       <c r="B6" s="182"/>
-      <c r="C6" s="185"/>
+      <c r="C6" s="188"/>
       <c r="D6" s="173"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="170"/>
       <c r="B7" s="182"/>
-      <c r="C7" s="185"/>
+      <c r="C7" s="188"/>
       <c r="D7" s="173"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="171"/>
       <c r="B8" s="183"/>
-      <c r="C8" s="186"/>
+      <c r="C8" s="189"/>
       <c r="D8" s="174"/>
       <c r="H8"/>
     </row>
@@ -21725,7 +21626,7 @@
       <c r="B9" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="184"/>
+      <c r="C9" s="187"/>
       <c r="D9" s="172"/>
       <c r="G9"/>
       <c r="H9"/>
@@ -21733,48 +21634,56 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="169"/>
       <c r="B10" s="182"/>
-      <c r="C10" s="185"/>
+      <c r="C10" s="188"/>
       <c r="D10" s="173"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="170"/>
       <c r="B11" s="182"/>
-      <c r="C11" s="185"/>
+      <c r="C11" s="188"/>
       <c r="D11" s="173"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="171"/>
       <c r="B12" s="183"/>
-      <c r="C12" s="186"/>
+      <c r="C12" s="189"/>
       <c r="D12" s="174"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="168"/>
       <c r="B13" s="181"/>
-      <c r="C13" s="184"/>
+      <c r="C13" s="187"/>
       <c r="D13" s="172"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="169"/>
       <c r="B14" s="182"/>
-      <c r="C14" s="185"/>
+      <c r="C14" s="188"/>
       <c r="D14" s="173"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="170"/>
       <c r="B15" s="182"/>
-      <c r="C15" s="185"/>
+      <c r="C15" s="188"/>
       <c r="D15" s="173"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="171"/>
       <c r="B16" s="183"/>
-      <c r="C16" s="186"/>
+      <c r="C16" s="189"/>
       <c r="D16" s="174"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -21783,14 +21692,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21820,7 +21721,7 @@
       <c r="B1" s="181" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="187"/>
+      <c r="C1" s="184"/>
       <c r="D1" s="181" t="s">
         <v>17</v>
       </c>
@@ -21828,20 +21729,20 @@
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="169"/>
       <c r="B2" s="182"/>
-      <c r="C2" s="188"/>
+      <c r="C2" s="185"/>
       <c r="D2" s="182"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="170"/>
       <c r="B3" s="182"/>
-      <c r="C3" s="188"/>
+      <c r="C3" s="185"/>
       <c r="D3" s="182"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="171"/>
       <c r="B4" s="183"/>
-      <c r="C4" s="189"/>
+      <c r="C4" s="186"/>
       <c r="D4" s="183"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -21851,7 +21752,7 @@
       <c r="B5" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="184"/>
+      <c r="C5" s="187"/>
       <c r="D5" s="172" t="s">
         <v>18</v>
       </c>
@@ -21860,19 +21761,19 @@
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="169"/>
       <c r="B6" s="182"/>
-      <c r="C6" s="185"/>
+      <c r="C6" s="188"/>
       <c r="D6" s="173"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="170"/>
       <c r="B7" s="182"/>
-      <c r="C7" s="185"/>
+      <c r="C7" s="188"/>
       <c r="D7" s="173"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="171"/>
       <c r="B8" s="183"/>
-      <c r="C8" s="186"/>
+      <c r="C8" s="189"/>
       <c r="D8" s="174"/>
       <c r="H8"/>
     </row>
@@ -21881,7 +21782,7 @@
       <c r="B9" s="181" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="184"/>
+      <c r="C9" s="187"/>
       <c r="D9" s="172" t="s">
         <v>19</v>
       </c>
@@ -21891,19 +21792,19 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="169"/>
       <c r="B10" s="182"/>
-      <c r="C10" s="185"/>
+      <c r="C10" s="188"/>
       <c r="D10" s="173"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="170"/>
       <c r="B11" s="182"/>
-      <c r="C11" s="185"/>
+      <c r="C11" s="188"/>
       <c r="D11" s="173"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="171"/>
       <c r="B12" s="183"/>
-      <c r="C12" s="186"/>
+      <c r="C12" s="189"/>
       <c r="D12" s="174"/>
       <c r="F12"/>
     </row>
@@ -21912,7 +21813,7 @@
       <c r="B13" s="181" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="184"/>
+      <c r="C13" s="187"/>
       <c r="D13" s="172" t="s">
         <v>20</v>
       </c>
@@ -21920,23 +21821,31 @@
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="169"/>
       <c r="B14" s="182"/>
-      <c r="C14" s="185"/>
+      <c r="C14" s="188"/>
       <c r="D14" s="173"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="170"/>
       <c r="B15" s="182"/>
-      <c r="C15" s="185"/>
+      <c r="C15" s="188"/>
       <c r="D15" s="173"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="171"/>
       <c r="B16" s="183"/>
-      <c r="C16" s="186"/>
+      <c r="C16" s="189"/>
       <c r="D16" s="174"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -21945,14 +21854,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -21982,7 +21883,7 @@
       <c r="B1" s="181" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="187"/>
+      <c r="C1" s="184"/>
       <c r="D1" s="172" t="s">
         <v>8</v>
       </c>
@@ -21990,19 +21891,19 @@
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="169"/>
       <c r="B2" s="182"/>
-      <c r="C2" s="188"/>
+      <c r="C2" s="185"/>
       <c r="D2" s="173"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="170"/>
       <c r="B3" s="182"/>
-      <c r="C3" s="188"/>
+      <c r="C3" s="185"/>
       <c r="D3" s="173"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="171"/>
       <c r="B4" s="183"/>
-      <c r="C4" s="189"/>
+      <c r="C4" s="186"/>
       <c r="D4" s="174"/>
       <c r="G4"/>
     </row>
@@ -22011,7 +21912,7 @@
       <c r="B5" s="181" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="184"/>
+      <c r="C5" s="187"/>
       <c r="D5" s="172" t="s">
         <v>7</v>
       </c>
@@ -22019,19 +21920,19 @@
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="169"/>
       <c r="B6" s="182"/>
-      <c r="C6" s="185"/>
+      <c r="C6" s="188"/>
       <c r="D6" s="173"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="170"/>
       <c r="B7" s="182"/>
-      <c r="C7" s="185"/>
+      <c r="C7" s="188"/>
       <c r="D7" s="173"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="171"/>
       <c r="B8" s="183"/>
-      <c r="C8" s="186"/>
+      <c r="C8" s="189"/>
       <c r="D8" s="174"/>
       <c r="H8"/>
     </row>
@@ -22040,7 +21941,7 @@
       <c r="B9" s="181" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="184"/>
+      <c r="C9" s="187"/>
       <c r="D9" s="172" t="s">
         <v>9</v>
       </c>
@@ -22048,19 +21949,19 @@
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="169"/>
       <c r="B10" s="182"/>
-      <c r="C10" s="185"/>
+      <c r="C10" s="188"/>
       <c r="D10" s="173"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="170"/>
       <c r="B11" s="182"/>
-      <c r="C11" s="185"/>
+      <c r="C11" s="188"/>
       <c r="D11" s="173"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="171"/>
       <c r="B12" s="183"/>
-      <c r="C12" s="186"/>
+      <c r="C12" s="189"/>
       <c r="D12" s="174"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -22068,29 +21969,37 @@
       <c r="B13" s="181" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="184"/>
+      <c r="C13" s="187"/>
       <c r="D13" s="172"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="169"/>
       <c r="B14" s="182"/>
-      <c r="C14" s="185"/>
+      <c r="C14" s="188"/>
       <c r="D14" s="173"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="170"/>
       <c r="B15" s="182"/>
-      <c r="C15" s="185"/>
+      <c r="C15" s="188"/>
       <c r="D15" s="173"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="171"/>
       <c r="B16" s="183"/>
-      <c r="C16" s="186"/>
+      <c r="C16" s="189"/>
       <c r="D16" s="174"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -22099,14 +22008,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22136,7 +22037,7 @@
       <c r="B1" s="181" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="187"/>
+      <c r="C1" s="184"/>
       <c r="D1" s="172" t="s">
         <v>31</v>
       </c>
@@ -22145,20 +22046,20 @@
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="169"/>
       <c r="B2" s="182"/>
-      <c r="C2" s="188"/>
+      <c r="C2" s="185"/>
       <c r="D2" s="173"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="170"/>
       <c r="B3" s="182"/>
-      <c r="C3" s="188"/>
+      <c r="C3" s="185"/>
       <c r="D3" s="173"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="171"/>
       <c r="B4" s="183"/>
-      <c r="C4" s="189"/>
+      <c r="C4" s="186"/>
       <c r="D4" s="174"/>
       <c r="F4"/>
     </row>
@@ -22167,7 +22068,7 @@
       <c r="B5" s="181" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="184"/>
+      <c r="C5" s="187"/>
       <c r="D5" s="172" t="s">
         <v>34</v>
       </c>
@@ -22175,20 +22076,20 @@
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="169"/>
       <c r="B6" s="182"/>
-      <c r="C6" s="185"/>
+      <c r="C6" s="188"/>
       <c r="D6" s="173"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="170"/>
       <c r="B7" s="182"/>
-      <c r="C7" s="185"/>
+      <c r="C7" s="188"/>
       <c r="D7" s="173"/>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="171"/>
       <c r="B8" s="183"/>
-      <c r="C8" s="186"/>
+      <c r="C8" s="189"/>
       <c r="D8" s="174"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -22196,7 +22097,7 @@
       <c r="B9" s="181" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="184"/>
+      <c r="C9" s="187"/>
       <c r="D9" s="172" t="s">
         <v>35</v>
       </c>
@@ -22205,25 +22106,25 @@
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="169"/>
       <c r="B10" s="182"/>
-      <c r="C10" s="185"/>
+      <c r="C10" s="188"/>
       <c r="D10" s="173"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="170"/>
       <c r="B11" s="182"/>
-      <c r="C11" s="185"/>
+      <c r="C11" s="188"/>
       <c r="D11" s="173"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="171"/>
       <c r="B12" s="183"/>
-      <c r="C12" s="186"/>
+      <c r="C12" s="189"/>
       <c r="D12" s="174"/>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="168"/>
       <c r="B13" s="181"/>
-      <c r="C13" s="184"/>
+      <c r="C13" s="187"/>
       <c r="D13" s="172" t="s">
         <v>36</v>
       </c>
@@ -22232,23 +22133,31 @@
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="169"/>
       <c r="B14" s="182"/>
-      <c r="C14" s="185"/>
+      <c r="C14" s="188"/>
       <c r="D14" s="173"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="170"/>
       <c r="B15" s="182"/>
-      <c r="C15" s="185"/>
+      <c r="C15" s="188"/>
       <c r="D15" s="173"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="171"/>
       <c r="B16" s="183"/>
-      <c r="C16" s="186"/>
+      <c r="C16" s="189"/>
       <c r="D16" s="174"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
@@ -22257,14 +22166,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -22414,13 +22315,13 @@
       <c r="H8" s="49"/>
     </row>
     <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="121" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="107"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
     </row>
     <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A12" s="65"/>
@@ -22430,165 +22331,156 @@
       <c r="E12" s="66"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="107" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="122" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="108"/>
-      <c r="B14" s="109" t="s">
+      <c r="A14" s="107"/>
+      <c r="B14" s="122" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="122"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="108"/>
-      <c r="B15" s="109" t="s">
+      <c r="A15" s="107"/>
+      <c r="B15" s="122" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="122"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="108"/>
-      <c r="B16" s="109" t="s">
+      <c r="A16" s="107"/>
+      <c r="B16" s="122" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="108"/>
-      <c r="B17" s="109" t="s">
+      <c r="A17" s="107"/>
+      <c r="B17" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="122"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="108" t="s">
+      <c r="A19" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="111" t="s">
+      <c r="B19" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="113"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="111"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="108"/>
-      <c r="B20" s="114"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="116"/>
+      <c r="A20" s="107"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="113"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="114"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="108" t="s">
+      <c r="A22" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="117" t="s">
+      <c r="B22" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="119"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="117"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="108"/>
-      <c r="B23" s="120"/>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="122"/>
+      <c r="A23" s="107"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="108"/>
-      <c r="B24" s="117" t="s">
+      <c r="A24" s="107"/>
+      <c r="B24" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="118"/>
-      <c r="D24" s="118"/>
-      <c r="E24" s="119"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="117"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="108"/>
-      <c r="B25" s="120"/>
-      <c r="C25" s="121"/>
-      <c r="D25" s="121"/>
-      <c r="E25" s="122"/>
+      <c r="A25" s="107"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="120"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="107" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="110" t="s">
+      <c r="B27" s="108" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="108"/>
-      <c r="B28" s="110"/>
-      <c r="C28" s="110"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="110"/>
+      <c r="A28" s="107"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="108"/>
-      <c r="B29" s="110"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="110"/>
+      <c r="A29" s="107"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="108" t="s">
+      <c r="A31" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="110" t="s">
+      <c r="B31" s="108" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="110"/>
-      <c r="D31" s="110"/>
-      <c r="E31" s="110"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="108"/>
+      <c r="E31" s="108"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="108"/>
-      <c r="B32" s="110"/>
-      <c r="C32" s="110"/>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
+      <c r="A32" s="107"/>
+      <c r="B32" s="108"/>
+      <c r="C32" s="108"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="108"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="108"/>
-      <c r="B33" s="110"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="110"/>
+      <c r="A33" s="107"/>
+      <c r="B33" s="108"/>
+      <c r="C33" s="108"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:E29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:E33"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:E20"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:E23"/>
-    <mergeCell ref="B24:E25"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B1:G1"/>
@@ -22599,6 +22491,15 @@
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:E29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:E33"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:E20"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:E23"/>
+    <mergeCell ref="B24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22750,14 +22651,14 @@
       <c r="F10" s="49"/>
     </row>
     <row r="12" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="107" t="s">
+      <c r="A12" s="121" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="107"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
     </row>
     <row r="13" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A13" s="65"/>
@@ -22768,180 +22669,173 @@
       <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="108" t="s">
+      <c r="A14" s="107" t="s">
         <v>162</v>
       </c>
       <c r="B14" s="70"/>
-      <c r="C14" s="109" t="s">
+      <c r="C14" s="122" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="122"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="108"/>
+      <c r="A15" s="107"/>
       <c r="B15" s="70"/>
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="122" t="s">
         <v>166</v>
       </c>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="122"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="108"/>
+      <c r="A16" s="107"/>
       <c r="B16" s="70"/>
-      <c r="C16" s="109" t="s">
+      <c r="C16" s="122" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
+      <c r="F16" s="122"/>
     </row>
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="108"/>
+      <c r="A17" s="107"/>
       <c r="B17" s="70"/>
-      <c r="C17" s="109" t="s">
+      <c r="C17" s="122" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="122"/>
     </row>
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="108"/>
+      <c r="A18" s="107"/>
       <c r="B18" s="70"/>
-      <c r="C18" s="109" t="s">
+      <c r="C18" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
+      <c r="D18" s="122"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="122"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
+      <c r="A20" s="107" t="s">
         <v>169</v>
       </c>
       <c r="B20" s="76"/>
-      <c r="C20" s="111" t="s">
+      <c r="C20" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="112"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="113"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="111"/>
     </row>
     <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="108"/>
+      <c r="A21" s="107"/>
       <c r="B21" s="77"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="115"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="116"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="114"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="107" t="s">
         <v>171</v>
       </c>
       <c r="B23" s="76"/>
-      <c r="C23" s="117" t="s">
+      <c r="C23" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="119"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="117"/>
     </row>
     <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="108"/>
+      <c r="A24" s="107"/>
       <c r="B24" s="77"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="121"/>
-      <c r="E24" s="121"/>
-      <c r="F24" s="122"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="120"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="108"/>
+      <c r="A25" s="107"/>
       <c r="B25" s="76"/>
-      <c r="C25" s="117" t="s">
+      <c r="C25" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="119"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="117"/>
     </row>
     <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="108"/>
+      <c r="A26" s="107"/>
       <c r="B26" s="77"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="121"/>
-      <c r="E26" s="121"/>
-      <c r="F26" s="122"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="120"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="108" t="s">
+      <c r="A28" s="107" t="s">
         <v>174</v>
       </c>
       <c r="B28" s="70"/>
-      <c r="C28" s="110" t="s">
+      <c r="C28" s="108" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="110"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="108"/>
     </row>
     <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="108"/>
+      <c r="A29" s="107"/>
       <c r="B29" s="70"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="110"/>
-      <c r="F29" s="110"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="108"/>
     </row>
     <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="108"/>
+      <c r="A30" s="107"/>
       <c r="B30" s="70"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="110"/>
-      <c r="E30" s="110"/>
-      <c r="F30" s="110"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="108"/>
     </row>
     <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="108" t="s">
+      <c r="A32" s="107" t="s">
         <v>176</v>
       </c>
       <c r="B32" s="70"/>
-      <c r="C32" s="110" t="s">
+      <c r="C32" s="108" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
-      <c r="F32" s="110"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="108"/>
     </row>
     <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="108"/>
+      <c r="A33" s="107"/>
       <c r="B33" s="70"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="110"/>
-      <c r="F33" s="110"/>
+      <c r="C33" s="108"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="108"/>
     </row>
     <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="108"/>
+      <c r="A34" s="107"/>
       <c r="B34" s="70"/>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
+      <c r="C34" s="108"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C28:F30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C32:F34"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="C23:F24"/>
-    <mergeCell ref="C25:F26"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="C3:F3"/>
@@ -22953,6 +22847,13 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C28:F30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C32:F34"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="C23:F24"/>
+    <mergeCell ref="C25:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23416,6 +23317,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="A41:E41"/>
@@ -23424,12 +23331,6 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B27:E27"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23441,7 +23342,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -23450,17 +23351,17 @@
     <col min="2" max="2" width="9.140625" style="6"/>
     <col min="3" max="3" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="7"/>
-    <col min="15" max="15" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="9.140625" style="7"/>
+    <col min="5" max="5" width="8.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="7" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="7" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="7" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="7" hidden="1" customWidth="1"/>
+    <col min="16" max="21" width="0" style="7" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="23" max="25" width="9.140625" style="7"/>
     <col min="26" max="26" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -23574,7 +23475,7 @@
       </c>
       <c r="D2" s="43">
         <f>SUM(E2:Z2)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="44"/>
@@ -23595,7 +23496,9 @@
         <v>2</v>
       </c>
       <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
+      <c r="V2" s="89">
+        <v>1</v>
+      </c>
       <c r="W2" s="89"/>
       <c r="X2" s="89"/>
       <c r="Y2" s="89"/>
@@ -23611,7 +23514,7 @@
       </c>
       <c r="D3" s="43">
         <f t="shared" ref="D3:D21" si="16">SUM(E3:Z3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="44"/>
@@ -23632,7 +23535,9 @@
         <v>1</v>
       </c>
       <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
+      <c r="V3" s="89">
+        <v>1</v>
+      </c>
       <c r="W3" s="89"/>
       <c r="X3" s="89"/>
       <c r="Y3" s="89"/>
@@ -23763,7 +23668,7 @@
       </c>
       <c r="D7" s="43">
         <f t="shared" si="16"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="22">
         <v>1</v>
@@ -23798,7 +23703,9 @@
       <c r="S7" s="89"/>
       <c r="T7" s="89"/>
       <c r="U7" s="89"/>
-      <c r="V7" s="89"/>
+      <c r="V7" s="89">
+        <v>1</v>
+      </c>
       <c r="W7" s="89"/>
       <c r="X7" s="89"/>
       <c r="Y7" s="89"/>
@@ -23913,7 +23820,7 @@
       </c>
       <c r="D11" s="43">
         <f t="shared" si="16"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E11" s="22">
         <v>1</v>
@@ -23948,8 +23855,12 @@
       <c r="S11" s="89"/>
       <c r="T11" s="89"/>
       <c r="U11" s="89"/>
-      <c r="V11" s="89"/>
-      <c r="W11" s="89"/>
+      <c r="V11" s="89">
+        <v>1</v>
+      </c>
+      <c r="W11" s="89">
+        <v>1</v>
+      </c>
       <c r="X11" s="89"/>
       <c r="Y11" s="89"/>
       <c r="Z11" s="89"/>
@@ -24029,7 +23940,7 @@
       </c>
       <c r="D14" s="43">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="44"/>
@@ -24048,7 +23959,9 @@
       <c r="S14" s="89"/>
       <c r="T14" s="89"/>
       <c r="U14" s="89"/>
-      <c r="V14" s="89"/>
+      <c r="V14" s="89">
+        <v>1</v>
+      </c>
       <c r="W14" s="89"/>
       <c r="X14" s="89"/>
       <c r="Y14" s="89"/>
@@ -24165,7 +24078,7 @@
       </c>
       <c r="D18" s="43">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="80"/>
@@ -24186,7 +24099,9 @@
         <v>1</v>
       </c>
       <c r="U18" s="89"/>
-      <c r="V18" s="89"/>
+      <c r="V18" s="89">
+        <v>1</v>
+      </c>
       <c r="W18" s="89"/>
       <c r="X18" s="89"/>
       <c r="Y18" s="89"/>
@@ -24231,7 +24146,7 @@
       </c>
       <c r="D20" s="43">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="80"/>
@@ -24252,7 +24167,9 @@
       <c r="S20" s="89"/>
       <c r="T20" s="89"/>
       <c r="U20" s="89"/>
-      <c r="V20" s="89"/>
+      <c r="V20" s="89">
+        <v>1</v>
+      </c>
       <c r="W20" s="89"/>
       <c r="X20" s="89"/>
       <c r="Y20" s="89"/>
@@ -24268,7 +24185,7 @@
       </c>
       <c r="D21" s="43">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="44"/>
@@ -24293,7 +24210,9 @@
       <c r="S21" s="89"/>
       <c r="T21" s="89"/>
       <c r="U21" s="89"/>
-      <c r="V21" s="89"/>
+      <c r="V21" s="89">
+        <v>1</v>
+      </c>
       <c r="W21" s="89"/>
       <c r="X21" s="89"/>
       <c r="Y21" s="89"/>
@@ -24365,12 +24284,12 @@
         <v>0</v>
       </c>
       <c r="V22" s="7">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f>SUM(V2:V21)</f>
+        <v>8</v>
       </c>
       <c r="W22" s="7">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22" s="7">
         <f t="shared" si="17"/>

</xml_diff>